<commit_message>
Paylines show on hit
Payline 1 to 3 to make
</commit_message>
<xml_diff>
--- a/Conceptual/Game rules + pay amounts.xlsx
+++ b/Conceptual/Game rules + pay amounts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andy_\OneDrive\Documenten\GitHub\slotmachine-practice\Conceptual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{833F8310-94FE-48D8-9BCA-D768A4C4792D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0738C253-917A-49F9-9806-9C243CE92086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31260" yWindow="-375" windowWidth="21600" windowHeight="11385" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28020" windowHeight="16440" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1806" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1808" uniqueCount="244">
   <si>
     <t>Symbols</t>
   </si>
@@ -1337,7 +1337,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="202">
+  <cellXfs count="204">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1692,6 +1692,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1749,16 +1771,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1770,27 +1786,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2392,7 +2398,7 @@
   <dimension ref="A1:N37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2433,12 +2439,12 @@
       <c r="H1" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="K1" s="175" t="s">
+      <c r="K1" s="183" t="s">
         <v>85</v>
       </c>
-      <c r="L1" s="176"/>
-      <c r="M1" s="176"/>
-      <c r="N1" s="177"/>
+      <c r="L1" s="184"/>
+      <c r="M1" s="184"/>
+      <c r="N1" s="185"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="163" t="s">
@@ -2503,11 +2509,11 @@
         <f>$H$19*Tabel1[[#This Row],[Pay 5X]]</f>
         <v>2</v>
       </c>
-      <c r="K3" s="181" t="s">
+      <c r="K3" s="189" t="s">
         <v>94</v>
       </c>
-      <c r="L3" s="171"/>
-      <c r="M3" s="171"/>
+      <c r="L3" s="179"/>
+      <c r="M3" s="179"/>
       <c r="N3" s="66"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -2571,12 +2577,12 @@
         <f>$H$19*Tabel1[[#This Row],[Pay 5X]]</f>
         <v>1.5</v>
       </c>
-      <c r="K5" s="182" t="s">
+      <c r="K5" s="190" t="s">
         <v>88</v>
       </c>
-      <c r="L5" s="183"/>
-      <c r="M5" s="183"/>
-      <c r="N5" s="184"/>
+      <c r="L5" s="191"/>
+      <c r="M5" s="191"/>
+      <c r="N5" s="192"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="163" t="s">
@@ -2756,12 +2762,12 @@
         <f>$H$19*Tabel1[[#This Row],[Pay 5X]]</f>
         <v>0.35</v>
       </c>
-      <c r="K10" s="178" t="s">
+      <c r="K10" s="186" t="s">
         <v>92</v>
       </c>
-      <c r="L10" s="179"/>
-      <c r="M10" s="179"/>
-      <c r="N10" s="180"/>
+      <c r="L10" s="187"/>
+      <c r="M10" s="187"/>
+      <c r="N10" s="188"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -2816,23 +2822,23 @@
       <c r="N13" s="66"/>
     </row>
     <row r="14" spans="1:14" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="K14" s="175" t="s">
+      <c r="K14" s="183" t="s">
         <v>95</v>
       </c>
-      <c r="L14" s="176"/>
-      <c r="M14" s="176"/>
-      <c r="N14" s="177"/>
+      <c r="L14" s="184"/>
+      <c r="M14" s="184"/>
+      <c r="N14" s="185"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="K15" s="168" t="s">
+      <c r="K15" s="176" t="s">
         <v>96</v>
       </c>
-      <c r="L15" s="169"/>
-      <c r="M15" s="169"/>
-      <c r="N15" s="170"/>
+      <c r="L15" s="177"/>
+      <c r="M15" s="177"/>
+      <c r="N15" s="178"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
@@ -2872,10 +2878,10 @@
       <c r="G18" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="H18" s="173" t="s">
+      <c r="H18" s="181" t="s">
         <v>102</v>
       </c>
-      <c r="I18" s="173"/>
+      <c r="I18" s="181"/>
       <c r="K18" s="42">
         <v>6</v>
       </c>
@@ -2911,11 +2917,11 @@
         <f>A16*A28*B19</f>
         <v>125</v>
       </c>
-      <c r="H19" s="174">
+      <c r="H19" s="182">
         <f>A16*A19*B24</f>
         <v>0.25</v>
       </c>
-      <c r="I19" s="174"/>
+      <c r="I19" s="182"/>
       <c r="J19" s="85"/>
       <c r="K19" s="42">
         <v>9</v>
@@ -3049,10 +3055,10 @@
       <c r="L23" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="M23" s="171" t="s">
+      <c r="M23" s="179" t="s">
         <v>56</v>
       </c>
-      <c r="N23" s="172"/>
+      <c r="N23" s="180"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="97">
@@ -3526,8 +3532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D90B50E7-CCC4-4662-92E0-5FAF72E473B1}">
   <dimension ref="B1:T105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3538,13 +3544,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="G1" s="188" t="s">
+      <c r="G1" s="201" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="188"/>
-      <c r="I1" s="188"/>
-      <c r="J1" s="188"/>
-      <c r="K1" s="188"/>
+      <c r="H1" s="201"/>
+      <c r="I1" s="201"/>
+      <c r="J1" s="201"/>
+      <c r="K1" s="201"/>
     </row>
     <row r="2" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G2" s="123">
@@ -3579,7 +3585,7 @@
       </c>
     </row>
     <row r="3" spans="2:20" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E3" s="197" t="s">
+      <c r="E3" s="202" t="s">
         <v>211</v>
       </c>
       <c r="F3" s="123">
@@ -3626,23 +3632,23 @@
       </c>
     </row>
     <row r="4" spans="2:20" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E4" s="197"/>
+      <c r="E4" s="202"/>
       <c r="F4" s="123">
         <v>75</v>
       </c>
-      <c r="G4" s="194" t="s">
+      <c r="G4" s="168" t="s">
         <v>208</v>
       </c>
-      <c r="H4" s="195" t="s">
+      <c r="H4" s="169" t="s">
         <v>221</v>
       </c>
-      <c r="I4" s="195" t="s">
+      <c r="I4" s="169" t="s">
         <v>222</v>
       </c>
-      <c r="J4" s="195" t="s">
+      <c r="J4" s="169" t="s">
         <v>223</v>
       </c>
-      <c r="K4" s="196" t="s">
+      <c r="K4" s="170" t="s">
         <v>224</v>
       </c>
       <c r="L4" s="123">
@@ -3651,19 +3657,19 @@
       <c r="N4" s="123">
         <v>75</v>
       </c>
-      <c r="O4" s="194">
-        <v>1</v>
-      </c>
-      <c r="P4" s="195">
-        <v>2</v>
-      </c>
-      <c r="Q4" s="195">
+      <c r="O4" s="168">
+        <v>1</v>
+      </c>
+      <c r="P4" s="169">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="169">
         <v>3</v>
       </c>
-      <c r="R4" s="195">
+      <c r="R4" s="169">
         <v>4</v>
       </c>
-      <c r="S4" s="196">
+      <c r="S4" s="170">
         <v>5</v>
       </c>
       <c r="T4" s="123">
@@ -3671,7 +3677,7 @@
       </c>
     </row>
     <row r="5" spans="2:20" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E5" s="197"/>
+      <c r="E5" s="202"/>
       <c r="F5" s="123">
         <v>125</v>
       </c>
@@ -3985,7 +3991,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
       <c r="C17" s="119" t="s">
         <v>207</v>
@@ -4000,11 +4006,11 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="198"/>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="198" t="s">
+    <row r="18" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="172"/>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B19" s="164" t="s">
         <v>156</v>
       </c>
       <c r="C19" s="121" t="s">
@@ -4016,15 +4022,15 @@
       <c r="G19" s="122" t="s">
         <v>220</v>
       </c>
-      <c r="H19" s="199" t="s">
+      <c r="H19" s="173" t="s">
         <v>215</v>
       </c>
-      <c r="I19" s="200" t="s">
+      <c r="I19" s="174" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="198"/>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B20" s="172"/>
       <c r="C20" s="117"/>
       <c r="D20" s="109" t="s">
         <v>221</v>
@@ -4034,15 +4040,15 @@
         <v>223</v>
       </c>
       <c r="G20" s="118"/>
-      <c r="H20" s="199" t="s">
+      <c r="H20" s="173" t="s">
         <v>216</v>
       </c>
-      <c r="I20" s="200" t="s">
+      <c r="I20" s="174" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="21" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="198"/>
+    <row r="21" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="172"/>
       <c r="C21" s="111"/>
       <c r="D21" s="112"/>
       <c r="E21" s="115" t="s">
@@ -4050,16 +4056,28 @@
       </c>
       <c r="F21" s="112"/>
       <c r="G21" s="113"/>
-      <c r="H21" s="199"/>
-      <c r="I21" s="200"/>
-    </row>
-    <row r="22" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="198"/>
-      <c r="H22" s="199"/>
-      <c r="I22" s="200"/>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="198" t="s">
+      <c r="H21" s="173"/>
+      <c r="I21" s="174"/>
+      <c r="K21" s="203" t="s">
+        <v>18</v>
+      </c>
+      <c r="L21" s="203" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="172"/>
+      <c r="H22" s="173"/>
+      <c r="I22" s="174"/>
+      <c r="K22" s="171">
+        <v>0</v>
+      </c>
+      <c r="L22" s="171">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B23" s="164" t="s">
         <v>157</v>
       </c>
       <c r="C23" s="105"/>
@@ -4069,15 +4087,21 @@
       </c>
       <c r="F23" s="106"/>
       <c r="G23" s="107"/>
-      <c r="H23" s="199" t="s">
+      <c r="H23" s="173" t="s">
         <v>215</v>
       </c>
-      <c r="I23" s="200" t="s">
+      <c r="I23" s="174" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="198"/>
+      <c r="K23" s="171">
+        <v>1</v>
+      </c>
+      <c r="L23" s="171">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B24" s="172"/>
       <c r="C24" s="117"/>
       <c r="D24" s="109" t="s">
         <v>221</v>
@@ -4087,15 +4111,21 @@
         <v>223</v>
       </c>
       <c r="G24" s="118"/>
-      <c r="H24" s="199" t="s">
+      <c r="H24" s="173" t="s">
         <v>216</v>
       </c>
-      <c r="I24" s="200" t="s">
+      <c r="I24" s="174" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="25" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="198"/>
+      <c r="K24" s="171">
+        <v>2</v>
+      </c>
+      <c r="L24" s="171">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="172"/>
       <c r="C25" s="119" t="s">
         <v>210</v>
       </c>
@@ -4105,16 +4135,24 @@
       <c r="G25" s="120" t="s">
         <v>228</v>
       </c>
-      <c r="H25" s="199"/>
-      <c r="I25" s="200"/>
-    </row>
-    <row r="26" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="198"/>
-      <c r="H26" s="199"/>
-      <c r="I26" s="200"/>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="198" t="s">
+      <c r="H25" s="173"/>
+      <c r="I25" s="174"/>
+      <c r="K25" s="171">
+        <v>3</v>
+      </c>
+      <c r="L25" s="171"/>
+    </row>
+    <row r="26" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="172"/>
+      <c r="H26" s="173"/>
+      <c r="I26" s="174"/>
+      <c r="K26" s="171">
+        <v>4</v>
+      </c>
+      <c r="L26" s="171"/>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B27" s="164" t="s">
         <v>158</v>
       </c>
       <c r="C27" s="105"/>
@@ -4128,15 +4166,19 @@
         <v>219</v>
       </c>
       <c r="G27" s="107"/>
-      <c r="H27" s="199" t="s">
+      <c r="H27" s="173" t="s">
         <v>215</v>
       </c>
-      <c r="I27" s="201" t="s">
+      <c r="I27" s="175" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B28" s="198"/>
+      <c r="K27" s="171">
+        <v>5</v>
+      </c>
+      <c r="L27" s="171"/>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B28" s="172"/>
       <c r="C28" s="108" t="s">
         <v>208</v>
       </c>
@@ -4146,30 +4188,34 @@
       <c r="G28" s="110" t="s">
         <v>224</v>
       </c>
-      <c r="H28" s="199" t="s">
+      <c r="H28" s="173" t="s">
         <v>216</v>
       </c>
-      <c r="I28" s="200" t="s">
+      <c r="I28" s="174" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="29" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="198"/>
+      <c r="K28" s="171">
+        <v>6</v>
+      </c>
+      <c r="L28" s="171"/>
+    </row>
+    <row r="29" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="172"/>
       <c r="C29" s="111"/>
       <c r="D29" s="112"/>
       <c r="E29" s="112"/>
       <c r="F29" s="112"/>
       <c r="G29" s="113"/>
-      <c r="H29" s="199"/>
-      <c r="I29" s="200"/>
-    </row>
-    <row r="30" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="198"/>
-      <c r="H30" s="199"/>
-      <c r="I30" s="200"/>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B31" s="198" t="s">
+      <c r="H29" s="173"/>
+      <c r="I29" s="174"/>
+    </row>
+    <row r="30" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="172"/>
+      <c r="H30" s="173"/>
+      <c r="I30" s="174"/>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B31" s="164" t="s">
         <v>159</v>
       </c>
       <c r="C31" s="124"/>
@@ -4177,15 +4223,15 @@
       <c r="E31" s="125"/>
       <c r="F31" s="125"/>
       <c r="G31" s="126"/>
-      <c r="H31" s="199" t="s">
+      <c r="H31" s="173" t="s">
         <v>215</v>
       </c>
-      <c r="I31" s="201" t="s">
+      <c r="I31" s="175" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B32" s="198"/>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B32" s="172"/>
       <c r="C32" s="108" t="s">
         <v>208</v>
       </c>
@@ -4195,15 +4241,15 @@
       <c r="G32" s="110" t="s">
         <v>224</v>
       </c>
-      <c r="H32" s="199" t="s">
+      <c r="H32" s="173" t="s">
         <v>216</v>
       </c>
-      <c r="I32" s="200" t="s">
+      <c r="I32" s="174" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="33" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="198"/>
+      <c r="B33" s="172"/>
       <c r="C33" s="127"/>
       <c r="D33" s="115" t="s">
         <v>225</v>
@@ -4215,16 +4261,16 @@
         <v>227</v>
       </c>
       <c r="G33" s="128"/>
-      <c r="H33" s="199"/>
-      <c r="I33" s="200"/>
+      <c r="H33" s="173"/>
+      <c r="I33" s="174"/>
     </row>
     <row r="34" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="198"/>
-      <c r="H34" s="199"/>
-      <c r="I34" s="200"/>
+      <c r="B34" s="172"/>
+      <c r="H34" s="173"/>
+      <c r="I34" s="174"/>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B35" s="198" t="s">
+      <c r="B35" s="164" t="s">
         <v>160</v>
       </c>
       <c r="C35" s="121" t="s">
@@ -4236,15 +4282,15 @@
       <c r="E35" s="106"/>
       <c r="F35" s="106"/>
       <c r="G35" s="107"/>
-      <c r="H35" s="199" t="s">
+      <c r="H35" s="173" t="s">
         <v>215</v>
       </c>
-      <c r="I35" s="200" t="s">
+      <c r="I35" s="174" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B36" s="198"/>
+      <c r="B36" s="172"/>
       <c r="C36" s="117"/>
       <c r="D36" s="114"/>
       <c r="E36" s="109" t="s">
@@ -4252,15 +4298,15 @@
       </c>
       <c r="F36" s="114"/>
       <c r="G36" s="118"/>
-      <c r="H36" s="199" t="s">
+      <c r="H36" s="173" t="s">
         <v>216</v>
       </c>
-      <c r="I36" s="200" t="s">
+      <c r="I36" s="174" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="37" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="198"/>
+      <c r="B37" s="172"/>
       <c r="C37" s="111"/>
       <c r="D37" s="112"/>
       <c r="E37" s="112"/>
@@ -4270,16 +4316,16 @@
       <c r="G37" s="120" t="s">
         <v>228</v>
       </c>
-      <c r="H37" s="199"/>
-      <c r="I37" s="200"/>
+      <c r="H37" s="173"/>
+      <c r="I37" s="174"/>
     </row>
     <row r="38" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="198"/>
-      <c r="H38" s="199"/>
-      <c r="I38" s="200"/>
+      <c r="B38" s="172"/>
+      <c r="H38" s="173"/>
+      <c r="I38" s="174"/>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B39" s="198" t="s">
+      <c r="B39" s="164" t="s">
         <v>161</v>
       </c>
       <c r="C39" s="105"/>
@@ -4291,15 +4337,15 @@
       <c r="G39" s="122" t="s">
         <v>220</v>
       </c>
-      <c r="H39" s="199" t="s">
+      <c r="H39" s="173" t="s">
         <v>215</v>
       </c>
-      <c r="I39" s="200" t="s">
+      <c r="I39" s="174" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B40" s="198"/>
+      <c r="B40" s="172"/>
       <c r="C40" s="117"/>
       <c r="D40" s="114"/>
       <c r="E40" s="109" t="s">
@@ -4307,15 +4353,15 @@
       </c>
       <c r="F40" s="114"/>
       <c r="G40" s="118"/>
-      <c r="H40" s="199" t="s">
+      <c r="H40" s="173" t="s">
         <v>216</v>
       </c>
-      <c r="I40" s="200" t="s">
+      <c r="I40" s="174" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="41" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="198"/>
+      <c r="B41" s="172"/>
       <c r="C41" s="119" t="s">
         <v>210</v>
       </c>
@@ -4325,16 +4371,16 @@
       <c r="E41" s="112"/>
       <c r="F41" s="112"/>
       <c r="G41" s="113"/>
-      <c r="H41" s="199"/>
-      <c r="I41" s="200"/>
+      <c r="H41" s="173"/>
+      <c r="I41" s="174"/>
     </row>
     <row r="42" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="198"/>
-      <c r="H42" s="199"/>
-      <c r="I42" s="200"/>
+      <c r="B42" s="172"/>
+      <c r="H42" s="173"/>
+      <c r="I42" s="174"/>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B43" s="198" t="s">
+      <c r="B43" s="164" t="s">
         <v>162</v>
       </c>
       <c r="C43" s="105"/>
@@ -4344,10 +4390,10 @@
         <v>219</v>
       </c>
       <c r="G43" s="107"/>
-      <c r="H43" s="199" t="s">
+      <c r="H43" s="173" t="s">
         <v>215</v>
       </c>
-      <c r="I43" s="201" t="s">
+      <c r="I43" s="175" t="s">
         <v>206</v>
       </c>
     </row>
@@ -4364,10 +4410,10 @@
       <c r="G44" s="110" t="s">
         <v>224</v>
       </c>
-      <c r="H44" s="199" t="s">
+      <c r="H44" s="173" t="s">
         <v>216</v>
       </c>
-      <c r="I44" s="200" t="s">
+      <c r="I44" s="174" t="s">
         <v>213</v>
       </c>
     </row>
@@ -4380,16 +4426,16 @@
       <c r="E45" s="112"/>
       <c r="F45" s="112"/>
       <c r="G45" s="113"/>
-      <c r="H45" s="199"/>
-      <c r="I45" s="200"/>
+      <c r="H45" s="173"/>
+      <c r="I45" s="174"/>
     </row>
     <row r="46" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="1"/>
-      <c r="H46" s="199"/>
-      <c r="I46" s="200"/>
+      <c r="H46" s="173"/>
+      <c r="I46" s="174"/>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B47" s="1" t="s">
+      <c r="B47" s="164" t="s">
         <v>163</v>
       </c>
       <c r="C47" s="105"/>
@@ -4399,10 +4445,10 @@
       <c r="E47" s="106"/>
       <c r="F47" s="106"/>
       <c r="G47" s="107"/>
-      <c r="H47" s="199" t="s">
+      <c r="H47" s="173" t="s">
         <v>215</v>
       </c>
-      <c r="I47" s="201" t="s">
+      <c r="I47" s="175" t="s">
         <v>206</v>
       </c>
     </row>
@@ -4419,10 +4465,10 @@
       <c r="G48" s="110" t="s">
         <v>224</v>
       </c>
-      <c r="H48" s="199" t="s">
+      <c r="H48" s="173" t="s">
         <v>216</v>
       </c>
-      <c r="I48" s="200" t="s">
+      <c r="I48" s="174" t="s">
         <v>213</v>
       </c>
     </row>
@@ -4435,16 +4481,16 @@
         <v>227</v>
       </c>
       <c r="G49" s="113"/>
-      <c r="H49" s="199"/>
-      <c r="I49" s="200"/>
+      <c r="H49" s="173"/>
+      <c r="I49" s="174"/>
     </row>
     <row r="50" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B50" s="1"/>
-      <c r="H50" s="199"/>
-      <c r="I50" s="200"/>
+      <c r="H50" s="173"/>
+      <c r="I50" s="174"/>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B51" s="1" t="s">
+      <c r="B51" s="164" t="s">
         <v>164</v>
       </c>
       <c r="C51" s="121" t="s">
@@ -4456,10 +4502,10 @@
       <c r="G51" s="122" t="s">
         <v>220</v>
       </c>
-      <c r="H51" s="199" t="s">
+      <c r="H51" s="173" t="s">
         <v>215</v>
       </c>
-      <c r="I51" s="200" t="s">
+      <c r="I51" s="174" t="s">
         <v>205</v>
       </c>
     </row>
@@ -4476,10 +4522,10 @@
         <v>223</v>
       </c>
       <c r="G52" s="118"/>
-      <c r="H52" s="199" t="s">
+      <c r="H52" s="173" t="s">
         <v>216</v>
       </c>
-      <c r="I52" s="200" t="s">
+      <c r="I52" s="174" t="s">
         <v>212</v>
       </c>
     </row>
@@ -4490,16 +4536,16 @@
       <c r="E53" s="112"/>
       <c r="F53" s="112"/>
       <c r="G53" s="113"/>
-      <c r="H53" s="199"/>
-      <c r="I53" s="200"/>
+      <c r="H53" s="173"/>
+      <c r="I53" s="174"/>
     </row>
     <row r="54" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B54" s="1"/>
-      <c r="H54" s="199"/>
-      <c r="I54" s="200"/>
+      <c r="H54" s="173"/>
+      <c r="I54" s="174"/>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B55" s="1" t="s">
+      <c r="B55" s="164" t="s">
         <v>165</v>
       </c>
       <c r="C55" s="105"/>
@@ -4507,10 +4553,10 @@
       <c r="E55" s="106"/>
       <c r="F55" s="106"/>
       <c r="G55" s="107"/>
-      <c r="H55" s="199" t="s">
+      <c r="H55" s="173" t="s">
         <v>215</v>
       </c>
-      <c r="I55" s="200" t="s">
+      <c r="I55" s="174" t="s">
         <v>207</v>
       </c>
     </row>
@@ -4527,10 +4573,10 @@
         <v>223</v>
       </c>
       <c r="G56" s="118"/>
-      <c r="H56" s="199" t="s">
+      <c r="H56" s="173" t="s">
         <v>216</v>
       </c>
-      <c r="I56" s="200" t="s">
+      <c r="I56" s="174" t="s">
         <v>214</v>
       </c>
     </row>
@@ -4545,16 +4591,16 @@
       <c r="G57" s="120" t="s">
         <v>228</v>
       </c>
-      <c r="H57" s="199"/>
-      <c r="I57" s="200"/>
+      <c r="H57" s="173"/>
+      <c r="I57" s="174"/>
     </row>
     <row r="58" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B58" s="1"/>
-      <c r="H58" s="199"/>
-      <c r="I58" s="200"/>
+      <c r="H58" s="173"/>
+      <c r="I58" s="174"/>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B59" s="1" t="s">
+      <c r="B59" s="164" t="s">
         <v>166</v>
       </c>
       <c r="C59" s="121" t="s">
@@ -4568,10 +4614,10 @@
       <c r="G59" s="122" t="s">
         <v>220</v>
       </c>
-      <c r="H59" s="199" t="s">
+      <c r="H59" s="173" t="s">
         <v>215</v>
       </c>
-      <c r="I59" s="200" t="s">
+      <c r="I59" s="174" t="s">
         <v>205</v>
       </c>
     </row>
@@ -4586,10 +4632,10 @@
         <v>223</v>
       </c>
       <c r="G60" s="118"/>
-      <c r="H60" s="199" t="s">
+      <c r="H60" s="173" t="s">
         <v>216</v>
       </c>
-      <c r="I60" s="200" t="s">
+      <c r="I60" s="174" t="s">
         <v>212</v>
       </c>
     </row>
@@ -4600,16 +4646,16 @@
       <c r="E61" s="112"/>
       <c r="F61" s="112"/>
       <c r="G61" s="113"/>
-      <c r="H61" s="199"/>
-      <c r="I61" s="200"/>
+      <c r="H61" s="173"/>
+      <c r="I61" s="174"/>
     </row>
     <row r="62" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B62" s="1"/>
-      <c r="H62" s="199"/>
-      <c r="I62" s="200"/>
+      <c r="H62" s="173"/>
+      <c r="I62" s="174"/>
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B63" s="1" t="s">
+      <c r="B63" s="164" t="s">
         <v>167</v>
       </c>
       <c r="C63" s="105"/>
@@ -4617,10 +4663,10 @@
       <c r="E63" s="106"/>
       <c r="F63" s="106"/>
       <c r="G63" s="107"/>
-      <c r="H63" s="199" t="s">
+      <c r="H63" s="173" t="s">
         <v>215</v>
       </c>
-      <c r="I63" s="200" t="s">
+      <c r="I63" s="174" t="s">
         <v>207</v>
       </c>
     </row>
@@ -4635,10 +4681,10 @@
         <v>223</v>
       </c>
       <c r="G64" s="118"/>
-      <c r="H64" s="199" t="s">
+      <c r="H64" s="173" t="s">
         <v>216</v>
       </c>
-      <c r="I64" s="200" t="s">
+      <c r="I64" s="174" t="s">
         <v>214</v>
       </c>
     </row>
@@ -4655,16 +4701,16 @@
       <c r="G65" s="120" t="s">
         <v>228</v>
       </c>
-      <c r="H65" s="199"/>
-      <c r="I65" s="200"/>
+      <c r="H65" s="173"/>
+      <c r="I65" s="174"/>
     </row>
     <row r="66" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B66" s="1"/>
-      <c r="H66" s="199"/>
-      <c r="I66" s="200"/>
+      <c r="H66" s="173"/>
+      <c r="I66" s="174"/>
     </row>
     <row r="67" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B67" s="1" t="s">
+      <c r="B67" s="164" t="s">
         <v>168</v>
       </c>
       <c r="C67" s="105"/>
@@ -4674,10 +4720,10 @@
       </c>
       <c r="F67" s="106"/>
       <c r="G67" s="107"/>
-      <c r="H67" s="199" t="s">
+      <c r="H67" s="173" t="s">
         <v>215</v>
       </c>
-      <c r="I67" s="201" t="s">
+      <c r="I67" s="175" t="s">
         <v>206</v>
       </c>
     </row>
@@ -4696,10 +4742,10 @@
       <c r="G68" s="110" t="s">
         <v>224</v>
       </c>
-      <c r="H68" s="199" t="s">
+      <c r="H68" s="173" t="s">
         <v>216</v>
       </c>
-      <c r="I68" s="200" t="s">
+      <c r="I68" s="174" t="s">
         <v>213</v>
       </c>
     </row>
@@ -4710,16 +4756,16 @@
       <c r="E69" s="112"/>
       <c r="F69" s="112"/>
       <c r="G69" s="113"/>
-      <c r="H69" s="199"/>
-      <c r="I69" s="200"/>
+      <c r="H69" s="173"/>
+      <c r="I69" s="174"/>
     </row>
     <row r="70" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B70" s="1"/>
-      <c r="H70" s="199"/>
-      <c r="I70" s="200"/>
+      <c r="H70" s="173"/>
+      <c r="I70" s="174"/>
     </row>
     <row r="71" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B71" s="1" t="s">
+      <c r="B71" s="164" t="s">
         <v>169</v>
       </c>
       <c r="C71" s="105"/>
@@ -4727,10 +4773,10 @@
       <c r="E71" s="106"/>
       <c r="F71" s="106"/>
       <c r="G71" s="107"/>
-      <c r="H71" s="199" t="s">
+      <c r="H71" s="173" t="s">
         <v>215</v>
       </c>
-      <c r="I71" s="201" t="s">
+      <c r="I71" s="175" t="s">
         <v>206</v>
       </c>
     </row>
@@ -4749,10 +4795,10 @@
       <c r="G72" s="110" t="s">
         <v>224</v>
       </c>
-      <c r="H72" s="199" t="s">
+      <c r="H72" s="173" t="s">
         <v>216</v>
       </c>
-      <c r="I72" s="200" t="s">
+      <c r="I72" s="174" t="s">
         <v>213</v>
       </c>
     </row>
@@ -4765,16 +4811,16 @@
       </c>
       <c r="F73" s="112"/>
       <c r="G73" s="113"/>
-      <c r="H73" s="199"/>
-      <c r="I73" s="200"/>
+      <c r="H73" s="173"/>
+      <c r="I73" s="174"/>
     </row>
     <row r="74" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B74" s="1"/>
-      <c r="H74" s="199"/>
-      <c r="I74" s="200"/>
+      <c r="H74" s="173"/>
+      <c r="I74" s="174"/>
     </row>
     <row r="75" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B75" s="1" t="s">
+      <c r="B75" s="164" t="s">
         <v>170</v>
       </c>
       <c r="C75" s="121" t="s">
@@ -4790,10 +4836,10 @@
       <c r="G75" s="122" t="s">
         <v>220</v>
       </c>
-      <c r="H75" s="199" t="s">
+      <c r="H75" s="173" t="s">
         <v>215</v>
       </c>
-      <c r="I75" s="200" t="s">
+      <c r="I75" s="174" t="s">
         <v>205</v>
       </c>
     </row>
@@ -4804,10 +4850,10 @@
       <c r="E76" s="114"/>
       <c r="F76" s="114"/>
       <c r="G76" s="118"/>
-      <c r="H76" s="199" t="s">
+      <c r="H76" s="173" t="s">
         <v>216</v>
       </c>
-      <c r="I76" s="200" t="s">
+      <c r="I76" s="174" t="s">
         <v>212</v>
       </c>
     </row>
@@ -4820,16 +4866,16 @@
       </c>
       <c r="F77" s="112"/>
       <c r="G77" s="113"/>
-      <c r="H77" s="199"/>
-      <c r="I77" s="200"/>
+      <c r="H77" s="173"/>
+      <c r="I77" s="174"/>
     </row>
     <row r="78" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B78" s="1"/>
-      <c r="H78" s="199"/>
-      <c r="I78" s="200"/>
+      <c r="H78" s="173"/>
+      <c r="I78" s="174"/>
     </row>
     <row r="79" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B79" s="1" t="s">
+      <c r="B79" s="164" t="s">
         <v>171</v>
       </c>
       <c r="C79" s="105"/>
@@ -4839,10 +4885,10 @@
       </c>
       <c r="F79" s="106"/>
       <c r="G79" s="107"/>
-      <c r="H79" s="199" t="s">
+      <c r="H79" s="173" t="s">
         <v>215</v>
       </c>
-      <c r="I79" s="200" t="s">
+      <c r="I79" s="174" t="s">
         <v>207</v>
       </c>
     </row>
@@ -4853,10 +4899,10 @@
       <c r="E80" s="114"/>
       <c r="F80" s="114"/>
       <c r="G80" s="118"/>
-      <c r="H80" s="199" t="s">
+      <c r="H80" s="173" t="s">
         <v>216</v>
       </c>
-      <c r="I80" s="200" t="s">
+      <c r="I80" s="174" t="s">
         <v>214</v>
       </c>
     </row>
@@ -4875,16 +4921,16 @@
       <c r="G81" s="120" t="s">
         <v>228</v>
       </c>
-      <c r="H81" s="199"/>
-      <c r="I81" s="200"/>
+      <c r="H81" s="173"/>
+      <c r="I81" s="174"/>
     </row>
     <row r="82" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B82" s="1"/>
-      <c r="H82" s="199"/>
-      <c r="I82" s="200"/>
+      <c r="H82" s="173"/>
+      <c r="I82" s="174"/>
     </row>
     <row r="83" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B83" s="1" t="s">
+      <c r="B83" s="164" t="s">
         <v>172</v>
       </c>
       <c r="C83" s="121" t="s">
@@ -4896,10 +4942,10 @@
       <c r="G83" s="122" t="s">
         <v>220</v>
       </c>
-      <c r="H83" s="199" t="s">
+      <c r="H83" s="173" t="s">
         <v>215</v>
       </c>
-      <c r="I83" s="200" t="s">
+      <c r="I83" s="174" t="s">
         <v>205</v>
       </c>
     </row>
@@ -4910,10 +4956,10 @@
       <c r="E84" s="114"/>
       <c r="F84" s="114"/>
       <c r="G84" s="118"/>
-      <c r="H84" s="199" t="s">
+      <c r="H84" s="173" t="s">
         <v>216</v>
       </c>
-      <c r="I84" s="200" t="s">
+      <c r="I84" s="174" t="s">
         <v>212</v>
       </c>
     </row>
@@ -4930,16 +4976,16 @@
         <v>227</v>
       </c>
       <c r="G85" s="113"/>
-      <c r="H85" s="199"/>
-      <c r="I85" s="200"/>
+      <c r="H85" s="173"/>
+      <c r="I85" s="174"/>
     </row>
     <row r="86" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B86" s="1"/>
-      <c r="H86" s="199"/>
-      <c r="I86" s="200"/>
+      <c r="H86" s="173"/>
+      <c r="I86" s="174"/>
     </row>
     <row r="87" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B87" s="1" t="s">
+      <c r="B87" s="164" t="s">
         <v>173</v>
       </c>
       <c r="C87" s="105"/>
@@ -4953,10 +4999,10 @@
         <v>219</v>
       </c>
       <c r="G87" s="107"/>
-      <c r="H87" s="199" t="s">
+      <c r="H87" s="173" t="s">
         <v>215</v>
       </c>
-      <c r="I87" s="200" t="s">
+      <c r="I87" s="174" t="s">
         <v>207</v>
       </c>
     </row>
@@ -4967,10 +5013,10 @@
       <c r="E88" s="114"/>
       <c r="F88" s="114"/>
       <c r="G88" s="118"/>
-      <c r="H88" s="199" t="s">
+      <c r="H88" s="173" t="s">
         <v>216</v>
       </c>
-      <c r="I88" s="200" t="s">
+      <c r="I88" s="174" t="s">
         <v>214</v>
       </c>
     </row>
@@ -4985,16 +5031,16 @@
       <c r="G89" s="120" t="s">
         <v>228</v>
       </c>
-      <c r="H89" s="199"/>
-      <c r="I89" s="200"/>
+      <c r="H89" s="173"/>
+      <c r="I89" s="174"/>
     </row>
     <row r="90" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B90" s="1"/>
-      <c r="H90" s="199"/>
-      <c r="I90" s="200"/>
+      <c r="H90" s="173"/>
+      <c r="I90" s="174"/>
     </row>
     <row r="91" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B91" s="1" t="s">
+      <c r="B91" s="164" t="s">
         <v>174</v>
       </c>
       <c r="C91" s="105"/>
@@ -5004,10 +5050,10 @@
       </c>
       <c r="F91" s="106"/>
       <c r="G91" s="107"/>
-      <c r="H91" s="199" t="s">
+      <c r="H91" s="173" t="s">
         <v>215</v>
       </c>
-      <c r="I91" s="201" t="s">
+      <c r="I91" s="175" t="s">
         <v>206</v>
       </c>
     </row>
@@ -5022,10 +5068,10 @@
       <c r="G92" s="110" t="s">
         <v>224</v>
       </c>
-      <c r="H92" s="199" t="s">
+      <c r="H92" s="173" t="s">
         <v>216</v>
       </c>
-      <c r="I92" s="200" t="s">
+      <c r="I92" s="174" t="s">
         <v>213</v>
       </c>
     </row>
@@ -5040,16 +5086,16 @@
         <v>227</v>
       </c>
       <c r="G93" s="113"/>
-      <c r="H93" s="199"/>
-      <c r="I93" s="200"/>
+      <c r="H93" s="173"/>
+      <c r="I93" s="174"/>
     </row>
     <row r="94" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B94" s="1"/>
-      <c r="H94" s="199"/>
-      <c r="I94" s="200"/>
+      <c r="H94" s="173"/>
+      <c r="I94" s="174"/>
     </row>
     <row r="95" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B95" s="1" t="s">
+      <c r="B95" s="164" t="s">
         <v>175</v>
       </c>
       <c r="C95" s="105"/>
@@ -5061,10 +5107,10 @@
         <v>219</v>
       </c>
       <c r="G95" s="107"/>
-      <c r="H95" s="199" t="s">
+      <c r="H95" s="173" t="s">
         <v>215</v>
       </c>
-      <c r="I95" s="201" t="s">
+      <c r="I95" s="175" t="s">
         <v>206</v>
       </c>
     </row>
@@ -5079,10 +5125,10 @@
       <c r="G96" s="110" t="s">
         <v>224</v>
       </c>
-      <c r="H96" s="199" t="s">
+      <c r="H96" s="173" t="s">
         <v>216</v>
       </c>
-      <c r="I96" s="200" t="s">
+      <c r="I96" s="174" t="s">
         <v>213</v>
       </c>
     </row>
@@ -5095,16 +5141,16 @@
       </c>
       <c r="F97" s="112"/>
       <c r="G97" s="113"/>
-      <c r="H97" s="199"/>
-      <c r="I97" s="200"/>
+      <c r="H97" s="173"/>
+      <c r="I97" s="174"/>
     </row>
     <row r="98" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B98" s="1"/>
-      <c r="H98" s="199"/>
-      <c r="I98" s="200"/>
+      <c r="H98" s="173"/>
+      <c r="I98" s="174"/>
     </row>
     <row r="99" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B99" s="1" t="s">
+      <c r="B99" s="164" t="s">
         <v>176</v>
       </c>
       <c r="C99" s="121" t="s">
@@ -5118,10 +5164,10 @@
       <c r="G99" s="122" t="s">
         <v>220</v>
       </c>
-      <c r="H99" s="199" t="s">
+      <c r="H99" s="173" t="s">
         <v>215</v>
       </c>
-      <c r="I99" s="200" t="s">
+      <c r="I99" s="174" t="s">
         <v>205</v>
       </c>
     </row>
@@ -5132,10 +5178,10 @@
       <c r="E100" s="114"/>
       <c r="F100" s="114"/>
       <c r="G100" s="118"/>
-      <c r="H100" s="199" t="s">
+      <c r="H100" s="173" t="s">
         <v>216</v>
       </c>
-      <c r="I100" s="200" t="s">
+      <c r="I100" s="174" t="s">
         <v>212</v>
       </c>
     </row>
@@ -5150,16 +5196,16 @@
         <v>227</v>
       </c>
       <c r="G101" s="113"/>
-      <c r="H101" s="199"/>
-      <c r="I101" s="200"/>
+      <c r="H101" s="173"/>
+      <c r="I101" s="174"/>
     </row>
     <row r="102" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B102" s="1"/>
-      <c r="H102" s="199"/>
-      <c r="I102" s="200"/>
+      <c r="H102" s="173"/>
+      <c r="I102" s="174"/>
     </row>
     <row r="103" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B103" s="1" t="s">
+      <c r="B103" s="164" t="s">
         <v>177</v>
       </c>
       <c r="C103" s="105"/>
@@ -5171,10 +5217,10 @@
         <v>219</v>
       </c>
       <c r="G103" s="107"/>
-      <c r="H103" s="199" t="s">
+      <c r="H103" s="173" t="s">
         <v>215</v>
       </c>
-      <c r="I103" s="200" t="s">
+      <c r="I103" s="174" t="s">
         <v>207</v>
       </c>
     </row>
@@ -5184,10 +5230,10 @@
       <c r="E104" s="114"/>
       <c r="F104" s="114"/>
       <c r="G104" s="118"/>
-      <c r="H104" s="199" t="s">
+      <c r="H104" s="173" t="s">
         <v>216</v>
       </c>
-      <c r="I104" s="200" t="s">
+      <c r="I104" s="174" t="s">
         <v>214</v>
       </c>
     </row>
@@ -5203,8 +5249,8 @@
       <c r="G105" s="120" t="s">
         <v>228</v>
       </c>
-      <c r="H105" s="199"/>
-      <c r="I105" s="200"/>
+      <c r="H105" s="173"/>
+      <c r="I105" s="174"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -5231,34 +5277,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="185">
-        <v>1</v>
-      </c>
-      <c r="C1" s="185"/>
-      <c r="D1" s="185"/>
-      <c r="E1" s="185"/>
-      <c r="F1" s="185"/>
-      <c r="H1" s="185">
-        <v>2</v>
-      </c>
-      <c r="I1" s="185"/>
-      <c r="J1" s="185"/>
-      <c r="K1" s="185"/>
-      <c r="L1" s="185"/>
-      <c r="N1" s="185">
+      <c r="B1" s="193">
+        <v>1</v>
+      </c>
+      <c r="C1" s="193"/>
+      <c r="D1" s="193"/>
+      <c r="E1" s="193"/>
+      <c r="F1" s="193"/>
+      <c r="H1" s="193">
+        <v>2</v>
+      </c>
+      <c r="I1" s="193"/>
+      <c r="J1" s="193"/>
+      <c r="K1" s="193"/>
+      <c r="L1" s="193"/>
+      <c r="N1" s="193">
         <v>3</v>
       </c>
-      <c r="O1" s="185"/>
-      <c r="P1" s="185"/>
-      <c r="Q1" s="185"/>
-      <c r="R1" s="185"/>
-      <c r="T1" s="185">
+      <c r="O1" s="193"/>
+      <c r="P1" s="193"/>
+      <c r="Q1" s="193"/>
+      <c r="R1" s="193"/>
+      <c r="T1" s="193">
         <v>4</v>
       </c>
-      <c r="U1" s="185"/>
-      <c r="V1" s="185"/>
-      <c r="W1" s="185"/>
-      <c r="X1" s="185"/>
+      <c r="U1" s="193"/>
+      <c r="V1" s="193"/>
+      <c r="W1" s="193"/>
+      <c r="X1" s="193"/>
     </row>
     <row r="2" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B2" s="121" t="s">
@@ -5481,37 +5527,37 @@
       <c r="X5" s="123"/>
     </row>
     <row r="6" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="186">
+      <c r="B6" s="194">
         <v>5</v>
       </c>
-      <c r="C6" s="186"/>
-      <c r="D6" s="186"/>
-      <c r="E6" s="186"/>
-      <c r="F6" s="186"/>
+      <c r="C6" s="194"/>
+      <c r="D6" s="194"/>
+      <c r="E6" s="194"/>
+      <c r="F6" s="194"/>
       <c r="G6" s="123"/>
-      <c r="H6" s="186">
+      <c r="H6" s="194">
         <v>6</v>
       </c>
-      <c r="I6" s="186"/>
-      <c r="J6" s="186"/>
-      <c r="K6" s="186"/>
-      <c r="L6" s="186"/>
+      <c r="I6" s="194"/>
+      <c r="J6" s="194"/>
+      <c r="K6" s="194"/>
+      <c r="L6" s="194"/>
       <c r="M6" s="123"/>
-      <c r="N6" s="186">
+      <c r="N6" s="194">
         <v>7</v>
       </c>
-      <c r="O6" s="186"/>
-      <c r="P6" s="186"/>
-      <c r="Q6" s="186"/>
-      <c r="R6" s="186"/>
+      <c r="O6" s="194"/>
+      <c r="P6" s="194"/>
+      <c r="Q6" s="194"/>
+      <c r="R6" s="194"/>
       <c r="S6" s="123"/>
-      <c r="T6" s="186">
+      <c r="T6" s="194">
         <v>8</v>
       </c>
-      <c r="U6" s="186"/>
-      <c r="V6" s="186"/>
-      <c r="W6" s="186"/>
-      <c r="X6" s="186"/>
+      <c r="U6" s="194"/>
+      <c r="V6" s="194"/>
+      <c r="W6" s="194"/>
+      <c r="X6" s="194"/>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B7" s="105" t="s">
@@ -5734,37 +5780,37 @@
       <c r="X10" s="123"/>
     </row>
     <row r="11" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="186">
+      <c r="B11" s="194">
         <v>9</v>
       </c>
-      <c r="C11" s="186"/>
-      <c r="D11" s="186"/>
-      <c r="E11" s="186"/>
-      <c r="F11" s="186"/>
+      <c r="C11" s="194"/>
+      <c r="D11" s="194"/>
+      <c r="E11" s="194"/>
+      <c r="F11" s="194"/>
       <c r="G11" s="123"/>
-      <c r="H11" s="186">
+      <c r="H11" s="194">
         <v>10</v>
       </c>
-      <c r="I11" s="186"/>
-      <c r="J11" s="186"/>
-      <c r="K11" s="186"/>
-      <c r="L11" s="186"/>
+      <c r="I11" s="194"/>
+      <c r="J11" s="194"/>
+      <c r="K11" s="194"/>
+      <c r="L11" s="194"/>
       <c r="M11" s="123"/>
-      <c r="N11" s="186">
+      <c r="N11" s="194">
         <v>11</v>
       </c>
-      <c r="O11" s="186"/>
-      <c r="P11" s="186"/>
-      <c r="Q11" s="186"/>
-      <c r="R11" s="186"/>
+      <c r="O11" s="194"/>
+      <c r="P11" s="194"/>
+      <c r="Q11" s="194"/>
+      <c r="R11" s="194"/>
       <c r="S11" s="123"/>
-      <c r="T11" s="186">
+      <c r="T11" s="194">
         <v>12</v>
       </c>
-      <c r="U11" s="186"/>
-      <c r="V11" s="186"/>
-      <c r="W11" s="186"/>
-      <c r="X11" s="186"/>
+      <c r="U11" s="194"/>
+      <c r="V11" s="194"/>
+      <c r="W11" s="194"/>
+      <c r="X11" s="194"/>
     </row>
     <row r="12" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B12" s="105" t="s">
@@ -5987,37 +6033,37 @@
       <c r="X15" s="123"/>
     </row>
     <row r="16" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="186">
+      <c r="B16" s="194">
         <v>13</v>
       </c>
-      <c r="C16" s="186"/>
-      <c r="D16" s="186"/>
-      <c r="E16" s="186"/>
-      <c r="F16" s="186"/>
+      <c r="C16" s="194"/>
+      <c r="D16" s="194"/>
+      <c r="E16" s="194"/>
+      <c r="F16" s="194"/>
       <c r="G16" s="123"/>
-      <c r="H16" s="186">
+      <c r="H16" s="194">
         <v>14</v>
       </c>
-      <c r="I16" s="186"/>
-      <c r="J16" s="186"/>
-      <c r="K16" s="186"/>
-      <c r="L16" s="186"/>
+      <c r="I16" s="194"/>
+      <c r="J16" s="194"/>
+      <c r="K16" s="194"/>
+      <c r="L16" s="194"/>
       <c r="M16" s="123"/>
-      <c r="N16" s="186">
+      <c r="N16" s="194">
         <v>15</v>
       </c>
-      <c r="O16" s="186"/>
-      <c r="P16" s="186"/>
-      <c r="Q16" s="186"/>
-      <c r="R16" s="186"/>
+      <c r="O16" s="194"/>
+      <c r="P16" s="194"/>
+      <c r="Q16" s="194"/>
+      <c r="R16" s="194"/>
       <c r="S16" s="123"/>
-      <c r="T16" s="186">
+      <c r="T16" s="194">
         <v>16</v>
       </c>
-      <c r="U16" s="186"/>
-      <c r="V16" s="186"/>
-      <c r="W16" s="186"/>
-      <c r="X16" s="186"/>
+      <c r="U16" s="194"/>
+      <c r="V16" s="194"/>
+      <c r="W16" s="194"/>
+      <c r="X16" s="194"/>
     </row>
     <row r="17" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B17" s="105" t="s">
@@ -6215,34 +6261,34 @@
       </c>
     </row>
     <row r="21" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="185">
+      <c r="B21" s="193">
         <v>17</v>
       </c>
-      <c r="C21" s="185"/>
-      <c r="D21" s="185"/>
-      <c r="E21" s="185"/>
-      <c r="F21" s="185"/>
-      <c r="H21" s="185">
+      <c r="C21" s="193"/>
+      <c r="D21" s="193"/>
+      <c r="E21" s="193"/>
+      <c r="F21" s="193"/>
+      <c r="H21" s="193">
         <v>18</v>
       </c>
-      <c r="I21" s="185"/>
-      <c r="J21" s="185"/>
-      <c r="K21" s="185"/>
-      <c r="L21" s="185"/>
-      <c r="N21" s="185">
+      <c r="I21" s="193"/>
+      <c r="J21" s="193"/>
+      <c r="K21" s="193"/>
+      <c r="L21" s="193"/>
+      <c r="N21" s="193">
         <v>19</v>
       </c>
-      <c r="O21" s="185"/>
-      <c r="P21" s="185"/>
-      <c r="Q21" s="185"/>
-      <c r="R21" s="185"/>
-      <c r="T21" s="185">
+      <c r="O21" s="193"/>
+      <c r="P21" s="193"/>
+      <c r="Q21" s="193"/>
+      <c r="R21" s="193"/>
+      <c r="T21" s="193">
         <v>20</v>
       </c>
-      <c r="U21" s="185"/>
-      <c r="V21" s="185"/>
-      <c r="W21" s="185"/>
-      <c r="X21" s="185"/>
+      <c r="U21" s="193"/>
+      <c r="V21" s="193"/>
+      <c r="W21" s="193"/>
+      <c r="X21" s="193"/>
     </row>
     <row r="22" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B22" s="105" t="s">
@@ -6431,34 +6477,34 @@
       </c>
     </row>
     <row r="26" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="185">
-        <v>21</v>
-      </c>
-      <c r="C26" s="185"/>
-      <c r="D26" s="185"/>
-      <c r="E26" s="185"/>
-      <c r="F26" s="185"/>
-      <c r="H26" s="185">
+      <c r="B26" s="193">
+        <v>21</v>
+      </c>
+      <c r="C26" s="193"/>
+      <c r="D26" s="193"/>
+      <c r="E26" s="193"/>
+      <c r="F26" s="193"/>
+      <c r="H26" s="193">
         <v>22</v>
       </c>
-      <c r="I26" s="185"/>
-      <c r="J26" s="185"/>
-      <c r="K26" s="185"/>
-      <c r="L26" s="185"/>
-      <c r="N26" s="185">
+      <c r="I26" s="193"/>
+      <c r="J26" s="193"/>
+      <c r="K26" s="193"/>
+      <c r="L26" s="193"/>
+      <c r="N26" s="193">
         <v>23</v>
       </c>
-      <c r="O26" s="185"/>
-      <c r="P26" s="185"/>
-      <c r="Q26" s="185"/>
-      <c r="R26" s="185"/>
-      <c r="T26" s="185">
+      <c r="O26" s="193"/>
+      <c r="P26" s="193"/>
+      <c r="Q26" s="193"/>
+      <c r="R26" s="193"/>
+      <c r="T26" s="193">
         <v>24</v>
       </c>
-      <c r="U26" s="185"/>
-      <c r="V26" s="185"/>
-      <c r="W26" s="185"/>
-      <c r="X26" s="185"/>
+      <c r="U26" s="193"/>
+      <c r="V26" s="193"/>
+      <c r="W26" s="193"/>
+      <c r="X26" s="193"/>
     </row>
     <row r="27" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B27" s="105" t="s">
@@ -6647,13 +6693,13 @@
       </c>
     </row>
     <row r="31" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="185">
+      <c r="B31" s="193">
         <v>25</v>
       </c>
-      <c r="C31" s="185"/>
-      <c r="D31" s="185"/>
-      <c r="E31" s="185"/>
-      <c r="F31" s="185"/>
+      <c r="C31" s="193"/>
+      <c r="D31" s="193"/>
+      <c r="E31" s="193"/>
+      <c r="F31" s="193"/>
       <c r="H31" s="154"/>
       <c r="I31" s="154"/>
       <c r="J31" s="154"/>
@@ -6740,22 +6786,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="H1:L1"/>
-    <mergeCell ref="N1:R1"/>
-    <mergeCell ref="T1:X1"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="H6:L6"/>
-    <mergeCell ref="N6:R6"/>
-    <mergeCell ref="T6:X6"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="H11:L11"/>
-    <mergeCell ref="N11:R11"/>
-    <mergeCell ref="T11:X11"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="H16:L16"/>
-    <mergeCell ref="N16:R16"/>
-    <mergeCell ref="T16:X16"/>
     <mergeCell ref="B31:F31"/>
     <mergeCell ref="B21:F21"/>
     <mergeCell ref="H21:L21"/>
@@ -6765,6 +6795,22 @@
     <mergeCell ref="H26:L26"/>
     <mergeCell ref="N26:R26"/>
     <mergeCell ref="T26:X26"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="H11:L11"/>
+    <mergeCell ref="N11:R11"/>
+    <mergeCell ref="T11:X11"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="H16:L16"/>
+    <mergeCell ref="N16:R16"/>
+    <mergeCell ref="T16:X16"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="H1:L1"/>
+    <mergeCell ref="N1:R1"/>
+    <mergeCell ref="T1:X1"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="H6:L6"/>
+    <mergeCell ref="N6:R6"/>
+    <mergeCell ref="T6:X6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7389,48 +7435,48 @@
       <c r="G9" s="151">
         <v>0.01</v>
       </c>
-      <c r="H9" s="189" t="s">
+      <c r="H9" s="196" t="s">
         <v>74</v>
       </c>
-      <c r="I9" s="189"/>
-      <c r="J9" s="189"/>
-      <c r="K9" s="189"/>
-      <c r="L9" s="189"/>
-      <c r="M9" s="189"/>
-      <c r="N9" s="189"/>
-      <c r="O9" s="189"/>
-      <c r="P9" s="189"/>
-      <c r="Q9" s="189"/>
+      <c r="I9" s="196"/>
+      <c r="J9" s="196"/>
+      <c r="K9" s="196"/>
+      <c r="L9" s="196"/>
+      <c r="M9" s="196"/>
+      <c r="N9" s="196"/>
+      <c r="O9" s="196"/>
+      <c r="P9" s="196"/>
+      <c r="Q9" s="196"/>
       <c r="S9" s="151">
         <v>0.01</v>
       </c>
-      <c r="T9" s="179" t="s">
+      <c r="T9" s="187" t="s">
         <v>75</v>
       </c>
-      <c r="U9" s="179"/>
-      <c r="V9" s="179"/>
-      <c r="W9" s="179"/>
-      <c r="X9" s="179"/>
-      <c r="Y9" s="179"/>
-      <c r="Z9" s="179"/>
-      <c r="AA9" s="179"/>
-      <c r="AB9" s="179"/>
-      <c r="AC9" s="179"/>
+      <c r="U9" s="187"/>
+      <c r="V9" s="187"/>
+      <c r="W9" s="187"/>
+      <c r="X9" s="187"/>
+      <c r="Y9" s="187"/>
+      <c r="Z9" s="187"/>
+      <c r="AA9" s="187"/>
+      <c r="AB9" s="187"/>
+      <c r="AC9" s="187"/>
       <c r="AE9" s="151">
         <v>0.01</v>
       </c>
-      <c r="AF9" s="179" t="s">
+      <c r="AF9" s="187" t="s">
         <v>76</v>
       </c>
-      <c r="AG9" s="179"/>
-      <c r="AH9" s="179"/>
-      <c r="AI9" s="179"/>
-      <c r="AJ9" s="179"/>
-      <c r="AK9" s="179"/>
-      <c r="AL9" s="179"/>
-      <c r="AM9" s="179"/>
-      <c r="AN9" s="179"/>
-      <c r="AO9" s="179"/>
+      <c r="AG9" s="187"/>
+      <c r="AH9" s="187"/>
+      <c r="AI9" s="187"/>
+      <c r="AJ9" s="187"/>
+      <c r="AK9" s="187"/>
+      <c r="AL9" s="187"/>
+      <c r="AM9" s="187"/>
+      <c r="AN9" s="187"/>
+      <c r="AO9" s="187"/>
     </row>
     <row r="10" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A10" s="101" t="s">
@@ -8720,44 +8766,44 @@
       <c r="G19" s="153">
         <v>0.03</v>
       </c>
-      <c r="H19" s="190"/>
-      <c r="I19" s="190"/>
-      <c r="J19" s="190"/>
-      <c r="K19" s="190"/>
-      <c r="L19" s="190"/>
-      <c r="M19" s="190"/>
-      <c r="N19" s="190"/>
-      <c r="O19" s="190"/>
-      <c r="P19" s="190"/>
-      <c r="Q19" s="190"/>
+      <c r="H19" s="195"/>
+      <c r="I19" s="195"/>
+      <c r="J19" s="195"/>
+      <c r="K19" s="195"/>
+      <c r="L19" s="195"/>
+      <c r="M19" s="195"/>
+      <c r="N19" s="195"/>
+      <c r="O19" s="195"/>
+      <c r="P19" s="195"/>
+      <c r="Q19" s="195"/>
       <c r="R19" s="152"/>
       <c r="S19" s="153">
         <v>0.03</v>
       </c>
-      <c r="T19" s="190"/>
-      <c r="U19" s="190"/>
-      <c r="V19" s="190"/>
-      <c r="W19" s="190"/>
-      <c r="X19" s="190"/>
-      <c r="Y19" s="190"/>
-      <c r="Z19" s="190"/>
-      <c r="AA19" s="190"/>
-      <c r="AB19" s="190"/>
-      <c r="AC19" s="190"/>
+      <c r="T19" s="195"/>
+      <c r="U19" s="195"/>
+      <c r="V19" s="195"/>
+      <c r="W19" s="195"/>
+      <c r="X19" s="195"/>
+      <c r="Y19" s="195"/>
+      <c r="Z19" s="195"/>
+      <c r="AA19" s="195"/>
+      <c r="AB19" s="195"/>
+      <c r="AC19" s="195"/>
       <c r="AD19" s="152"/>
       <c r="AE19" s="151">
         <v>0.03</v>
       </c>
-      <c r="AF19" s="190"/>
-      <c r="AG19" s="190"/>
-      <c r="AH19" s="190"/>
-      <c r="AI19" s="190"/>
-      <c r="AJ19" s="190"/>
-      <c r="AK19" s="190"/>
-      <c r="AL19" s="190"/>
-      <c r="AM19" s="190"/>
-      <c r="AN19" s="190"/>
-      <c r="AO19" s="190"/>
+      <c r="AF19" s="195"/>
+      <c r="AG19" s="195"/>
+      <c r="AH19" s="195"/>
+      <c r="AI19" s="195"/>
+      <c r="AJ19" s="195"/>
+      <c r="AK19" s="195"/>
+      <c r="AL19" s="195"/>
+      <c r="AM19" s="195"/>
+      <c r="AN19" s="195"/>
+      <c r="AO19" s="195"/>
     </row>
     <row r="20" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A20" s="97">
@@ -11212,44 +11258,44 @@
       <c r="G39" s="153">
         <v>0.1</v>
       </c>
-      <c r="H39" s="190"/>
-      <c r="I39" s="190"/>
-      <c r="J39" s="190"/>
-      <c r="K39" s="190"/>
-      <c r="L39" s="190"/>
-      <c r="M39" s="190"/>
-      <c r="N39" s="190"/>
-      <c r="O39" s="190"/>
-      <c r="P39" s="190"/>
-      <c r="Q39" s="190"/>
+      <c r="H39" s="195"/>
+      <c r="I39" s="195"/>
+      <c r="J39" s="195"/>
+      <c r="K39" s="195"/>
+      <c r="L39" s="195"/>
+      <c r="M39" s="195"/>
+      <c r="N39" s="195"/>
+      <c r="O39" s="195"/>
+      <c r="P39" s="195"/>
+      <c r="Q39" s="195"/>
       <c r="R39" s="152"/>
       <c r="S39" s="153">
         <v>0.1</v>
       </c>
-      <c r="T39" s="190"/>
-      <c r="U39" s="190"/>
-      <c r="V39" s="190"/>
-      <c r="W39" s="190"/>
-      <c r="X39" s="190"/>
-      <c r="Y39" s="190"/>
-      <c r="Z39" s="190"/>
-      <c r="AA39" s="190"/>
-      <c r="AB39" s="190"/>
-      <c r="AC39" s="190"/>
+      <c r="T39" s="195"/>
+      <c r="U39" s="195"/>
+      <c r="V39" s="195"/>
+      <c r="W39" s="195"/>
+      <c r="X39" s="195"/>
+      <c r="Y39" s="195"/>
+      <c r="Z39" s="195"/>
+      <c r="AA39" s="195"/>
+      <c r="AB39" s="195"/>
+      <c r="AC39" s="195"/>
       <c r="AD39" s="152"/>
       <c r="AE39" s="151">
         <v>0.1</v>
       </c>
-      <c r="AF39" s="190"/>
-      <c r="AG39" s="190"/>
-      <c r="AH39" s="190"/>
-      <c r="AI39" s="190"/>
-      <c r="AJ39" s="190"/>
-      <c r="AK39" s="190"/>
-      <c r="AL39" s="190"/>
-      <c r="AM39" s="190"/>
-      <c r="AN39" s="190"/>
-      <c r="AO39" s="190"/>
+      <c r="AF39" s="195"/>
+      <c r="AG39" s="195"/>
+      <c r="AH39" s="195"/>
+      <c r="AI39" s="195"/>
+      <c r="AJ39" s="195"/>
+      <c r="AK39" s="195"/>
+      <c r="AL39" s="195"/>
+      <c r="AM39" s="195"/>
+      <c r="AN39" s="195"/>
+      <c r="AO39" s="195"/>
     </row>
     <row r="40" spans="7:41" x14ac:dyDescent="0.25">
       <c r="G40" s="158">
@@ -13692,44 +13738,44 @@
       <c r="G59" s="153">
         <v>0.5</v>
       </c>
-      <c r="H59" s="190"/>
-      <c r="I59" s="190"/>
-      <c r="J59" s="190"/>
-      <c r="K59" s="190"/>
-      <c r="L59" s="190"/>
-      <c r="M59" s="190"/>
-      <c r="N59" s="190"/>
-      <c r="O59" s="190"/>
-      <c r="P59" s="190"/>
-      <c r="Q59" s="190"/>
+      <c r="H59" s="195"/>
+      <c r="I59" s="195"/>
+      <c r="J59" s="195"/>
+      <c r="K59" s="195"/>
+      <c r="L59" s="195"/>
+      <c r="M59" s="195"/>
+      <c r="N59" s="195"/>
+      <c r="O59" s="195"/>
+      <c r="P59" s="195"/>
+      <c r="Q59" s="195"/>
       <c r="R59" s="152"/>
       <c r="S59" s="153">
         <v>0.5</v>
       </c>
-      <c r="T59" s="190"/>
-      <c r="U59" s="190"/>
-      <c r="V59" s="190"/>
-      <c r="W59" s="190"/>
-      <c r="X59" s="190"/>
-      <c r="Y59" s="190"/>
-      <c r="Z59" s="190"/>
-      <c r="AA59" s="190"/>
-      <c r="AB59" s="190"/>
-      <c r="AC59" s="190"/>
+      <c r="T59" s="195"/>
+      <c r="U59" s="195"/>
+      <c r="V59" s="195"/>
+      <c r="W59" s="195"/>
+      <c r="X59" s="195"/>
+      <c r="Y59" s="195"/>
+      <c r="Z59" s="195"/>
+      <c r="AA59" s="195"/>
+      <c r="AB59" s="195"/>
+      <c r="AC59" s="195"/>
       <c r="AD59" s="152"/>
       <c r="AE59" s="151">
         <v>0.5</v>
       </c>
-      <c r="AF59" s="190"/>
-      <c r="AG59" s="190"/>
-      <c r="AH59" s="190"/>
-      <c r="AI59" s="190"/>
-      <c r="AJ59" s="190"/>
-      <c r="AK59" s="190"/>
-      <c r="AL59" s="190"/>
-      <c r="AM59" s="190"/>
-      <c r="AN59" s="190"/>
-      <c r="AO59" s="190"/>
+      <c r="AF59" s="195"/>
+      <c r="AG59" s="195"/>
+      <c r="AH59" s="195"/>
+      <c r="AI59" s="195"/>
+      <c r="AJ59" s="195"/>
+      <c r="AK59" s="195"/>
+      <c r="AL59" s="195"/>
+      <c r="AM59" s="195"/>
+      <c r="AN59" s="195"/>
+      <c r="AO59" s="195"/>
     </row>
     <row r="60" spans="7:41" x14ac:dyDescent="0.25">
       <c r="G60" s="158">
@@ -14930,6 +14976,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="H9:Q9"/>
+    <mergeCell ref="T9:AC9"/>
+    <mergeCell ref="AF9:AO9"/>
+    <mergeCell ref="AF19:AO19"/>
+    <mergeCell ref="AF39:AO39"/>
     <mergeCell ref="AF59:AO59"/>
     <mergeCell ref="T19:AC19"/>
     <mergeCell ref="T39:AC39"/>
@@ -14937,11 +14988,6 @@
     <mergeCell ref="H19:Q19"/>
     <mergeCell ref="H39:Q39"/>
     <mergeCell ref="H59:Q59"/>
-    <mergeCell ref="H9:Q9"/>
-    <mergeCell ref="T9:AC9"/>
-    <mergeCell ref="AF9:AO9"/>
-    <mergeCell ref="AF19:AO19"/>
-    <mergeCell ref="AF39:AO39"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="AF20:AO28 AF60:AO68 AF40:AO48">
@@ -18156,34 +18202,34 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="185">
-        <v>1</v>
-      </c>
-      <c r="C1" s="185"/>
-      <c r="D1" s="185"/>
-      <c r="E1" s="185"/>
-      <c r="F1" s="185"/>
-      <c r="H1" s="185">
-        <v>2</v>
-      </c>
-      <c r="I1" s="185"/>
-      <c r="J1" s="185"/>
-      <c r="K1" s="185"/>
-      <c r="L1" s="185"/>
-      <c r="N1" s="185">
+      <c r="B1" s="193">
+        <v>1</v>
+      </c>
+      <c r="C1" s="193"/>
+      <c r="D1" s="193"/>
+      <c r="E1" s="193"/>
+      <c r="F1" s="193"/>
+      <c r="H1" s="193">
+        <v>2</v>
+      </c>
+      <c r="I1" s="193"/>
+      <c r="J1" s="193"/>
+      <c r="K1" s="193"/>
+      <c r="L1" s="193"/>
+      <c r="N1" s="193">
         <v>3</v>
       </c>
-      <c r="O1" s="185"/>
-      <c r="P1" s="185"/>
-      <c r="Q1" s="185"/>
-      <c r="R1" s="185"/>
-      <c r="T1" s="185">
+      <c r="O1" s="193"/>
+      <c r="P1" s="193"/>
+      <c r="Q1" s="193"/>
+      <c r="R1" s="193"/>
+      <c r="T1" s="193">
         <v>4</v>
       </c>
-      <c r="U1" s="185"/>
-      <c r="V1" s="185"/>
-      <c r="W1" s="185"/>
-      <c r="X1" s="185"/>
+      <c r="U1" s="193"/>
+      <c r="V1" s="193"/>
+      <c r="W1" s="193"/>
+      <c r="X1" s="193"/>
     </row>
     <row r="2" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B2" s="39"/>
@@ -18252,34 +18298,34 @@
       <c r="X4" s="46"/>
     </row>
     <row r="6" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="185">
+      <c r="B6" s="193">
         <v>5</v>
       </c>
-      <c r="C6" s="185"/>
-      <c r="D6" s="185"/>
-      <c r="E6" s="185"/>
-      <c r="F6" s="185"/>
-      <c r="H6" s="185">
+      <c r="C6" s="193"/>
+      <c r="D6" s="193"/>
+      <c r="E6" s="193"/>
+      <c r="F6" s="193"/>
+      <c r="H6" s="193">
         <v>6</v>
       </c>
-      <c r="I6" s="185"/>
-      <c r="J6" s="185"/>
-      <c r="K6" s="185"/>
-      <c r="L6" s="185"/>
-      <c r="N6" s="185">
+      <c r="I6" s="193"/>
+      <c r="J6" s="193"/>
+      <c r="K6" s="193"/>
+      <c r="L6" s="193"/>
+      <c r="N6" s="193">
         <v>7</v>
       </c>
-      <c r="O6" s="185"/>
-      <c r="P6" s="185"/>
-      <c r="Q6" s="185"/>
-      <c r="R6" s="185"/>
-      <c r="T6" s="185">
+      <c r="O6" s="193"/>
+      <c r="P6" s="193"/>
+      <c r="Q6" s="193"/>
+      <c r="R6" s="193"/>
+      <c r="T6" s="193">
         <v>8</v>
       </c>
-      <c r="U6" s="185"/>
-      <c r="V6" s="185"/>
-      <c r="W6" s="185"/>
-      <c r="X6" s="185"/>
+      <c r="U6" s="193"/>
+      <c r="V6" s="193"/>
+      <c r="W6" s="193"/>
+      <c r="X6" s="193"/>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B7" s="39"/>
@@ -18348,34 +18394,34 @@
       <c r="X9" s="59"/>
     </row>
     <row r="11" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="185">
+      <c r="B11" s="193">
         <v>9</v>
       </c>
-      <c r="C11" s="185"/>
-      <c r="D11" s="185"/>
-      <c r="E11" s="185"/>
-      <c r="F11" s="185"/>
-      <c r="H11" s="185">
+      <c r="C11" s="193"/>
+      <c r="D11" s="193"/>
+      <c r="E11" s="193"/>
+      <c r="F11" s="193"/>
+      <c r="H11" s="193">
         <v>10</v>
       </c>
-      <c r="I11" s="185"/>
-      <c r="J11" s="185"/>
-      <c r="K11" s="185"/>
-      <c r="L11" s="185"/>
-      <c r="N11" s="185">
+      <c r="I11" s="193"/>
+      <c r="J11" s="193"/>
+      <c r="K11" s="193"/>
+      <c r="L11" s="193"/>
+      <c r="N11" s="193">
         <v>11</v>
       </c>
-      <c r="O11" s="185"/>
-      <c r="P11" s="185"/>
-      <c r="Q11" s="185"/>
-      <c r="R11" s="185"/>
-      <c r="T11" s="185">
+      <c r="O11" s="193"/>
+      <c r="P11" s="193"/>
+      <c r="Q11" s="193"/>
+      <c r="R11" s="193"/>
+      <c r="T11" s="193">
         <v>12</v>
       </c>
-      <c r="U11" s="185"/>
-      <c r="V11" s="185"/>
-      <c r="W11" s="185"/>
-      <c r="X11" s="185"/>
+      <c r="U11" s="193"/>
+      <c r="V11" s="193"/>
+      <c r="W11" s="193"/>
+      <c r="X11" s="193"/>
     </row>
     <row r="12" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B12" s="39"/>
@@ -18444,34 +18490,34 @@
       <c r="X14" s="46"/>
     </row>
     <row r="16" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="185">
+      <c r="B16" s="193">
         <v>13</v>
       </c>
-      <c r="C16" s="185"/>
-      <c r="D16" s="185"/>
-      <c r="E16" s="185"/>
-      <c r="F16" s="185"/>
-      <c r="H16" s="185">
+      <c r="C16" s="193"/>
+      <c r="D16" s="193"/>
+      <c r="E16" s="193"/>
+      <c r="F16" s="193"/>
+      <c r="H16" s="193">
         <v>14</v>
       </c>
-      <c r="I16" s="185"/>
-      <c r="J16" s="185"/>
-      <c r="K16" s="185"/>
-      <c r="L16" s="185"/>
-      <c r="N16" s="185">
+      <c r="I16" s="193"/>
+      <c r="J16" s="193"/>
+      <c r="K16" s="193"/>
+      <c r="L16" s="193"/>
+      <c r="N16" s="193">
         <v>15</v>
       </c>
-      <c r="O16" s="185"/>
-      <c r="P16" s="185"/>
-      <c r="Q16" s="185"/>
-      <c r="R16" s="185"/>
-      <c r="T16" s="185">
+      <c r="O16" s="193"/>
+      <c r="P16" s="193"/>
+      <c r="Q16" s="193"/>
+      <c r="R16" s="193"/>
+      <c r="T16" s="193">
         <v>16</v>
       </c>
-      <c r="U16" s="185"/>
-      <c r="V16" s="185"/>
-      <c r="W16" s="185"/>
-      <c r="X16" s="185"/>
+      <c r="U16" s="193"/>
+      <c r="V16" s="193"/>
+      <c r="W16" s="193"/>
+      <c r="X16" s="193"/>
     </row>
     <row r="17" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B17" s="39"/>
@@ -18540,34 +18586,34 @@
       <c r="X19" s="46"/>
     </row>
     <row r="21" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="185">
+      <c r="B21" s="193">
         <v>17</v>
       </c>
-      <c r="C21" s="185"/>
-      <c r="D21" s="185"/>
-      <c r="E21" s="185"/>
-      <c r="F21" s="185"/>
-      <c r="H21" s="185">
+      <c r="C21" s="193"/>
+      <c r="D21" s="193"/>
+      <c r="E21" s="193"/>
+      <c r="F21" s="193"/>
+      <c r="H21" s="193">
         <v>18</v>
       </c>
-      <c r="I21" s="185"/>
-      <c r="J21" s="185"/>
-      <c r="K21" s="185"/>
-      <c r="L21" s="185"/>
-      <c r="N21" s="185">
+      <c r="I21" s="193"/>
+      <c r="J21" s="193"/>
+      <c r="K21" s="193"/>
+      <c r="L21" s="193"/>
+      <c r="N21" s="193">
         <v>19</v>
       </c>
-      <c r="O21" s="185"/>
-      <c r="P21" s="185"/>
-      <c r="Q21" s="185"/>
-      <c r="R21" s="185"/>
-      <c r="T21" s="185">
+      <c r="O21" s="193"/>
+      <c r="P21" s="193"/>
+      <c r="Q21" s="193"/>
+      <c r="R21" s="193"/>
+      <c r="T21" s="193">
         <v>20</v>
       </c>
-      <c r="U21" s="185"/>
-      <c r="V21" s="185"/>
-      <c r="W21" s="185"/>
-      <c r="X21" s="185"/>
+      <c r="U21" s="193"/>
+      <c r="V21" s="193"/>
+      <c r="W21" s="193"/>
+      <c r="X21" s="193"/>
     </row>
     <row r="22" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B22" s="39"/>
@@ -18636,34 +18682,34 @@
       <c r="X24" s="46"/>
     </row>
     <row r="26" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="185">
-        <v>21</v>
-      </c>
-      <c r="C26" s="185"/>
-      <c r="D26" s="185"/>
-      <c r="E26" s="185"/>
-      <c r="F26" s="185"/>
-      <c r="H26" s="185">
+      <c r="B26" s="193">
+        <v>21</v>
+      </c>
+      <c r="C26" s="193"/>
+      <c r="D26" s="193"/>
+      <c r="E26" s="193"/>
+      <c r="F26" s="193"/>
+      <c r="H26" s="193">
         <v>22</v>
       </c>
-      <c r="I26" s="185"/>
-      <c r="J26" s="185"/>
-      <c r="K26" s="185"/>
-      <c r="L26" s="185"/>
-      <c r="N26" s="185">
+      <c r="I26" s="193"/>
+      <c r="J26" s="193"/>
+      <c r="K26" s="193"/>
+      <c r="L26" s="193"/>
+      <c r="N26" s="193">
         <v>23</v>
       </c>
-      <c r="O26" s="185"/>
-      <c r="P26" s="185"/>
-      <c r="Q26" s="185"/>
-      <c r="R26" s="185"/>
-      <c r="T26" s="185">
+      <c r="O26" s="193"/>
+      <c r="P26" s="193"/>
+      <c r="Q26" s="193"/>
+      <c r="R26" s="193"/>
+      <c r="T26" s="193">
         <v>24</v>
       </c>
-      <c r="U26" s="185"/>
-      <c r="V26" s="185"/>
-      <c r="W26" s="185"/>
-      <c r="X26" s="185"/>
+      <c r="U26" s="193"/>
+      <c r="V26" s="193"/>
+      <c r="W26" s="193"/>
+      <c r="X26" s="193"/>
     </row>
     <row r="27" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B27" s="39"/>
@@ -18732,13 +18778,13 @@
       <c r="X29" s="46"/>
     </row>
     <row r="31" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="185">
+      <c r="B31" s="193">
         <v>25</v>
       </c>
-      <c r="C31" s="185"/>
-      <c r="D31" s="185"/>
-      <c r="E31" s="185"/>
-      <c r="F31" s="185"/>
+      <c r="C31" s="193"/>
+      <c r="D31" s="193"/>
+      <c r="E31" s="193"/>
+      <c r="F31" s="193"/>
     </row>
     <row r="32" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B32" s="39"/>
@@ -18763,22 +18809,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="H1:L1"/>
-    <mergeCell ref="N1:R1"/>
-    <mergeCell ref="T1:X1"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="H6:L6"/>
-    <mergeCell ref="N6:R6"/>
-    <mergeCell ref="T6:X6"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="H11:L11"/>
-    <mergeCell ref="N11:R11"/>
-    <mergeCell ref="T11:X11"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="H26:L26"/>
-    <mergeCell ref="N26:R26"/>
-    <mergeCell ref="T26:X26"/>
     <mergeCell ref="B31:F31"/>
     <mergeCell ref="T16:X16"/>
     <mergeCell ref="B21:F21"/>
@@ -18788,6 +18818,22 @@
     <mergeCell ref="B16:F16"/>
     <mergeCell ref="H16:L16"/>
     <mergeCell ref="N16:R16"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="H11:L11"/>
+    <mergeCell ref="N11:R11"/>
+    <mergeCell ref="T11:X11"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="H26:L26"/>
+    <mergeCell ref="N26:R26"/>
+    <mergeCell ref="T26:X26"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="H1:L1"/>
+    <mergeCell ref="N1:R1"/>
+    <mergeCell ref="T1:X1"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="H6:L6"/>
+    <mergeCell ref="N6:R6"/>
+    <mergeCell ref="T6:X6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -18811,40 +18857,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="191" t="s">
+      <c r="A1" s="197" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="192"/>
-      <c r="C1" s="192"/>
-      <c r="D1" s="193"/>
-      <c r="F1" s="191" t="s">
+      <c r="B1" s="198"/>
+      <c r="C1" s="198"/>
+      <c r="D1" s="199"/>
+      <c r="F1" s="197" t="s">
         <v>58</v>
       </c>
-      <c r="G1" s="192"/>
-      <c r="H1" s="193"/>
+      <c r="G1" s="198"/>
+      <c r="H1" s="199"/>
       <c r="I1" s="47"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="168" t="s">
+      <c r="A2" s="176" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="169"/>
-      <c r="C2" s="169"/>
-      <c r="D2" s="170"/>
-      <c r="F2" s="168" t="s">
+      <c r="B2" s="177"/>
+      <c r="C2" s="177"/>
+      <c r="D2" s="178"/>
+      <c r="F2" s="176" t="s">
         <v>59</v>
       </c>
-      <c r="G2" s="169"/>
-      <c r="H2" s="170"/>
+      <c r="G2" s="177"/>
+      <c r="H2" s="178"/>
       <c r="I2" s="47"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="168" t="s">
+      <c r="A3" s="176" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="169"/>
-      <c r="C3" s="169"/>
-      <c r="D3" s="170"/>
+      <c r="B3" s="177"/>
+      <c r="C3" s="177"/>
+      <c r="D3" s="178"/>
       <c r="F3" s="13" t="s">
         <v>60</v>
       </c>
@@ -18996,10 +19042,10 @@
       <c r="B12" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="171" t="s">
+      <c r="C12" s="179" t="s">
         <v>56</v>
       </c>
-      <c r="D12" s="172"/>
+      <c r="D12" s="180"/>
       <c r="F12" s="13" t="s">
         <v>67</v>
       </c>
@@ -19018,11 +19064,11 @@
       <c r="H13" s="66"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="168" t="s">
+      <c r="A14" s="176" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="169"/>
-      <c r="C14" s="169"/>
+      <c r="B14" s="177"/>
+      <c r="C14" s="177"/>
       <c r="D14" s="66"/>
       <c r="F14" s="13" t="s">
         <v>68</v>
@@ -19031,11 +19077,11 @@
       <c r="H14" s="66"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="168" t="s">
+      <c r="A15" s="176" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="169"/>
-      <c r="C15" s="169"/>
+      <c r="B15" s="177"/>
+      <c r="C15" s="177"/>
       <c r="D15" s="66"/>
       <c r="F15" s="13" t="s">
         <v>69</v>
@@ -19097,8 +19143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DF38956-FDBF-4967-97AF-72744B5458AB}">
   <dimension ref="A1:AC174"/>
   <sheetViews>
-    <sheetView topLeftCell="A142" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:L172"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H191" sqref="H191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19230,11 +19276,11 @@
       <c r="P4" s="123" t="s">
         <v>21</v>
       </c>
-      <c r="Q4" s="187" t="s">
+      <c r="Q4" s="200" t="s">
         <v>185</v>
       </c>
-      <c r="R4" s="187"/>
-      <c r="S4" s="187"/>
+      <c r="R4" s="200"/>
+      <c r="S4" s="200"/>
     </row>
     <row r="5" spans="5:29" x14ac:dyDescent="0.25">
       <c r="E5" s="5"/>
@@ -19495,13 +19541,13 @@
       <c r="Q19" s="123"/>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A20" s="188" t="s">
+      <c r="A20" s="201" t="s">
         <v>200</v>
       </c>
-      <c r="B20" s="188"/>
-      <c r="C20" s="188"/>
-      <c r="D20" s="188"/>
-      <c r="E20" s="188"/>
+      <c r="B20" s="201"/>
+      <c r="C20" s="201"/>
+      <c r="D20" s="201"/>
+      <c r="E20" s="201"/>
       <c r="G20" s="1"/>
       <c r="M20" s="123"/>
       <c r="N20" s="123"/>

</xml_diff>

<commit_message>
adding payline 1 to 3
</commit_message>
<xml_diff>
--- a/Conceptual/Game rules + pay amounts.xlsx
+++ b/Conceptual/Game rules + pay amounts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andy_\OneDrive\Documenten\GitHub\slotmachine-practice\Conceptual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0738C253-917A-49F9-9806-9C243CE92086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A229B4-176F-4BB3-B381-F8C757C0823C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28020" windowHeight="16440" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28020" windowHeight="16440" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -1337,7 +1337,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="204">
+  <cellXfs count="212">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1714,6 +1714,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1771,10 +1774,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1795,7 +1798,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2056,14 +2080,14 @@
       </fill>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2079,7 +2103,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabel1" displayName="Tabel1" ref="A1:H13" totalsRowShown="0" headerRowDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabel1" displayName="Tabel1" ref="A1:H13" totalsRowShown="0" headerRowDxfId="36">
   <autoFilter ref="A1:H13" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H13">
     <sortCondition ref="B1:B13"/>
@@ -2439,12 +2463,12 @@
       <c r="H1" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="K1" s="183" t="s">
+      <c r="K1" s="184" t="s">
         <v>85</v>
       </c>
-      <c r="L1" s="184"/>
-      <c r="M1" s="184"/>
-      <c r="N1" s="185"/>
+      <c r="L1" s="185"/>
+      <c r="M1" s="185"/>
+      <c r="N1" s="186"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="163" t="s">
@@ -2509,11 +2533,11 @@
         <f>$H$19*Tabel1[[#This Row],[Pay 5X]]</f>
         <v>2</v>
       </c>
-      <c r="K3" s="189" t="s">
+      <c r="K3" s="190" t="s">
         <v>94</v>
       </c>
-      <c r="L3" s="179"/>
-      <c r="M3" s="179"/>
+      <c r="L3" s="180"/>
+      <c r="M3" s="180"/>
       <c r="N3" s="66"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -2577,12 +2601,12 @@
         <f>$H$19*Tabel1[[#This Row],[Pay 5X]]</f>
         <v>1.5</v>
       </c>
-      <c r="K5" s="190" t="s">
+      <c r="K5" s="191" t="s">
         <v>88</v>
       </c>
-      <c r="L5" s="191"/>
-      <c r="M5" s="191"/>
-      <c r="N5" s="192"/>
+      <c r="L5" s="192"/>
+      <c r="M5" s="192"/>
+      <c r="N5" s="193"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="163" t="s">
@@ -2762,12 +2786,12 @@
         <f>$H$19*Tabel1[[#This Row],[Pay 5X]]</f>
         <v>0.35</v>
       </c>
-      <c r="K10" s="186" t="s">
+      <c r="K10" s="187" t="s">
         <v>92</v>
       </c>
-      <c r="L10" s="187"/>
-      <c r="M10" s="187"/>
-      <c r="N10" s="188"/>
+      <c r="L10" s="188"/>
+      <c r="M10" s="188"/>
+      <c r="N10" s="189"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -2822,23 +2846,23 @@
       <c r="N13" s="66"/>
     </row>
     <row r="14" spans="1:14" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="K14" s="183" t="s">
+      <c r="K14" s="184" t="s">
         <v>95</v>
       </c>
-      <c r="L14" s="184"/>
-      <c r="M14" s="184"/>
-      <c r="N14" s="185"/>
+      <c r="L14" s="185"/>
+      <c r="M14" s="185"/>
+      <c r="N14" s="186"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="K15" s="176" t="s">
+      <c r="K15" s="177" t="s">
         <v>96</v>
       </c>
-      <c r="L15" s="177"/>
-      <c r="M15" s="177"/>
-      <c r="N15" s="178"/>
+      <c r="L15" s="178"/>
+      <c r="M15" s="178"/>
+      <c r="N15" s="179"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
@@ -2878,10 +2902,10 @@
       <c r="G18" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="H18" s="181" t="s">
+      <c r="H18" s="182" t="s">
         <v>102</v>
       </c>
-      <c r="I18" s="181"/>
+      <c r="I18" s="182"/>
       <c r="K18" s="42">
         <v>6</v>
       </c>
@@ -2917,11 +2941,11 @@
         <f>A16*A28*B19</f>
         <v>125</v>
       </c>
-      <c r="H19" s="182">
+      <c r="H19" s="183">
         <f>A16*A19*B24</f>
         <v>0.25</v>
       </c>
-      <c r="I19" s="182"/>
+      <c r="I19" s="183"/>
       <c r="J19" s="85"/>
       <c r="K19" s="42">
         <v>9</v>
@@ -3055,10 +3079,10 @@
       <c r="L23" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="M23" s="179" t="s">
+      <c r="M23" s="180" t="s">
         <v>56</v>
       </c>
-      <c r="N23" s="180"/>
+      <c r="N23" s="181"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="97">
@@ -3516,7 +3540,7 @@
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="F2:H10">
-    <cfRule type="cellIs" dxfId="36" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="37" priority="1" operator="greaterThan">
       <formula>$H$19</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3532,8 +3556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D90B50E7-CCC4-4662-92E0-5FAF72E473B1}">
   <dimension ref="B1:T105"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3544,13 +3568,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="G1" s="201" t="s">
+      <c r="G1" s="202" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="201"/>
-      <c r="I1" s="201"/>
-      <c r="J1" s="201"/>
-      <c r="K1" s="201"/>
+      <c r="H1" s="202"/>
+      <c r="I1" s="202"/>
+      <c r="J1" s="202"/>
+      <c r="K1" s="202"/>
     </row>
     <row r="2" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G2" s="123">
@@ -3568,24 +3592,16 @@
       <c r="K2" s="123">
         <v>270</v>
       </c>
-      <c r="O2" s="123">
-        <v>30</v>
-      </c>
-      <c r="P2" s="123">
-        <v>90</v>
-      </c>
-      <c r="Q2" s="123">
-        <v>150</v>
-      </c>
-      <c r="R2" s="123">
-        <v>210</v>
-      </c>
-      <c r="S2" s="123">
-        <v>270</v>
-      </c>
+      <c r="O2" s="210">
+        <v>1</v>
+      </c>
+      <c r="P2" s="210"/>
+      <c r="Q2" s="210"/>
+      <c r="R2" s="210"/>
+      <c r="S2" s="210"/>
     </row>
     <row r="3" spans="2:20" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E3" s="202" t="s">
+      <c r="E3" s="203" t="s">
         <v>211</v>
       </c>
       <c r="F3" s="123">
@@ -3609,30 +3625,27 @@
       <c r="L3" s="131">
         <v>300</v>
       </c>
-      <c r="N3" s="123">
-        <v>25</v>
-      </c>
-      <c r="O3" s="105">
-        <v>1</v>
-      </c>
-      <c r="P3" s="106">
-        <v>2</v>
-      </c>
-      <c r="Q3" s="106">
-        <v>3</v>
-      </c>
-      <c r="R3" s="106">
-        <v>4</v>
-      </c>
-      <c r="S3" s="107">
-        <v>5</v>
-      </c>
-      <c r="T3" s="131">
-        <v>300</v>
-      </c>
+      <c r="N3" s="205">
+        <v>1</v>
+      </c>
+      <c r="O3" s="206">
+        <f>N3/3</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="P3" s="209">
+        <f>O3/9</f>
+        <v>3.7037037037037035E-2</v>
+      </c>
+      <c r="Q3" s="211">
+        <f>1.3*25</f>
+        <v>32.5</v>
+      </c>
+      <c r="R3" s="106"/>
+      <c r="S3" s="107"/>
+      <c r="T3" s="131"/>
     </row>
     <row r="4" spans="2:20" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E4" s="202"/>
+      <c r="E4" s="203"/>
       <c r="F4" s="123">
         <v>75</v>
       </c>
@@ -3654,30 +3667,24 @@
       <c r="L4" s="123">
         <v>300</v>
       </c>
-      <c r="N4" s="123">
-        <v>75</v>
-      </c>
-      <c r="O4" s="168">
-        <v>1</v>
+      <c r="N4" s="204"/>
+      <c r="O4" s="207">
+        <f>O3*2</f>
+        <v>0.66666666666666663</v>
       </c>
       <c r="P4" s="169">
-        <v>2</v>
+        <f>P3*880</f>
+        <v>32.592592592592588</v>
       </c>
       <c r="Q4" s="169">
-        <v>3</v>
-      </c>
-      <c r="R4" s="169">
-        <v>4</v>
-      </c>
-      <c r="S4" s="170">
         <v>5</v>
       </c>
-      <c r="T4" s="123">
-        <v>300</v>
-      </c>
+      <c r="R4" s="169"/>
+      <c r="S4" s="170"/>
+      <c r="T4" s="123"/>
     </row>
     <row r="5" spans="2:20" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E5" s="202"/>
+      <c r="E5" s="203"/>
       <c r="F5" s="123">
         <v>125</v>
       </c>
@@ -3699,27 +3706,16 @@
       <c r="L5" s="123">
         <v>300</v>
       </c>
-      <c r="N5" s="123">
-        <v>125</v>
-      </c>
-      <c r="O5" s="111">
-        <v>1</v>
-      </c>
-      <c r="P5" s="112">
-        <v>2</v>
-      </c>
-      <c r="Q5" s="112">
-        <v>3</v>
-      </c>
-      <c r="R5" s="112">
-        <v>4</v>
-      </c>
-      <c r="S5" s="113">
-        <v>5</v>
-      </c>
-      <c r="T5" s="123">
-        <v>300</v>
-      </c>
+      <c r="N5" s="204"/>
+      <c r="O5" s="208">
+        <f>O3*3</f>
+        <v>1</v>
+      </c>
+      <c r="P5" s="112"/>
+      <c r="Q5" s="112"/>
+      <c r="R5" s="112"/>
+      <c r="S5" s="113"/>
+      <c r="T5" s="123"/>
     </row>
     <row r="6" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
@@ -3978,7 +3974,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
       <c r="C16" s="117"/>
       <c r="D16" s="114"/>
@@ -3991,7 +3987,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
       <c r="C17" s="119" t="s">
         <v>207</v>
@@ -4005,11 +4001,21 @@
       <c r="K17">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O17" s="124"/>
+      <c r="P17" s="125"/>
+      <c r="Q17" s="125"/>
+      <c r="R17" s="125"/>
+      <c r="S17" s="126"/>
+    </row>
+    <row r="18" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="172"/>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O18" s="117"/>
+      <c r="P18" s="114"/>
+      <c r="Q18" s="114"/>
+      <c r="R18" s="114"/>
+      <c r="S18" s="118"/>
+    </row>
+    <row r="19" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="164" t="s">
         <v>156</v>
       </c>
@@ -4028,8 +4034,13 @@
       <c r="I19" s="174" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O19" s="127"/>
+      <c r="P19" s="130"/>
+      <c r="Q19" s="130"/>
+      <c r="R19" s="130"/>
+      <c r="S19" s="128"/>
+    </row>
+    <row r="20" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B20" s="172"/>
       <c r="C20" s="117"/>
       <c r="D20" s="109" t="s">
@@ -4047,7 +4058,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="21" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="172"/>
       <c r="C21" s="111"/>
       <c r="D21" s="112"/>
@@ -4058,14 +4069,14 @@
       <c r="G21" s="113"/>
       <c r="H21" s="173"/>
       <c r="I21" s="174"/>
-      <c r="K21" s="203" t="s">
+      <c r="K21" s="176" t="s">
         <v>18</v>
       </c>
-      <c r="L21" s="203" t="s">
+      <c r="L21" s="176" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="22" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="172"/>
       <c r="H22" s="173"/>
       <c r="I22" s="174"/>
@@ -4076,7 +4087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B23" s="164" t="s">
         <v>157</v>
       </c>
@@ -4100,7 +4111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B24" s="172"/>
       <c r="C24" s="117"/>
       <c r="D24" s="109" t="s">
@@ -4124,7 +4135,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="172"/>
       <c r="C25" s="119" t="s">
         <v>210</v>
@@ -4142,7 +4153,7 @@
       </c>
       <c r="L25" s="171"/>
     </row>
-    <row r="26" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="172"/>
       <c r="H26" s="173"/>
       <c r="I26" s="174"/>
@@ -4151,7 +4162,7 @@
       </c>
       <c r="L26" s="171"/>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B27" s="164" t="s">
         <v>158</v>
       </c>
@@ -4177,7 +4188,7 @@
       </c>
       <c r="L27" s="171"/>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B28" s="172"/>
       <c r="C28" s="108" t="s">
         <v>208</v>
@@ -4199,7 +4210,7 @@
       </c>
       <c r="L28" s="171"/>
     </row>
-    <row r="29" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="172"/>
       <c r="C29" s="111"/>
       <c r="D29" s="112"/>
@@ -4209,12 +4220,12 @@
       <c r="H29" s="173"/>
       <c r="I29" s="174"/>
     </row>
-    <row r="30" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="172"/>
       <c r="H30" s="173"/>
       <c r="I30" s="174"/>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B31" s="164" t="s">
         <v>159</v>
       </c>
@@ -4230,7 +4241,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B32" s="172"/>
       <c r="C32" s="108" t="s">
         <v>208</v>
@@ -5253,9 +5264,11 @@
       <c r="I105" s="174"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="E3:E5"/>
     <mergeCell ref="G1:K1"/>
+    <mergeCell ref="N3:N5"/>
+    <mergeCell ref="O2:S2"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5277,34 +5290,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="193">
-        <v>1</v>
-      </c>
-      <c r="C1" s="193"/>
-      <c r="D1" s="193"/>
-      <c r="E1" s="193"/>
-      <c r="F1" s="193"/>
-      <c r="H1" s="193">
-        <v>2</v>
-      </c>
-      <c r="I1" s="193"/>
-      <c r="J1" s="193"/>
-      <c r="K1" s="193"/>
-      <c r="L1" s="193"/>
-      <c r="N1" s="193">
+      <c r="B1" s="194">
+        <v>1</v>
+      </c>
+      <c r="C1" s="194"/>
+      <c r="D1" s="194"/>
+      <c r="E1" s="194"/>
+      <c r="F1" s="194"/>
+      <c r="H1" s="194">
+        <v>2</v>
+      </c>
+      <c r="I1" s="194"/>
+      <c r="J1" s="194"/>
+      <c r="K1" s="194"/>
+      <c r="L1" s="194"/>
+      <c r="N1" s="194">
         <v>3</v>
       </c>
-      <c r="O1" s="193"/>
-      <c r="P1" s="193"/>
-      <c r="Q1" s="193"/>
-      <c r="R1" s="193"/>
-      <c r="T1" s="193">
+      <c r="O1" s="194"/>
+      <c r="P1" s="194"/>
+      <c r="Q1" s="194"/>
+      <c r="R1" s="194"/>
+      <c r="T1" s="194">
         <v>4</v>
       </c>
-      <c r="U1" s="193"/>
-      <c r="V1" s="193"/>
-      <c r="W1" s="193"/>
-      <c r="X1" s="193"/>
+      <c r="U1" s="194"/>
+      <c r="V1" s="194"/>
+      <c r="W1" s="194"/>
+      <c r="X1" s="194"/>
     </row>
     <row r="2" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B2" s="121" t="s">
@@ -5527,37 +5540,37 @@
       <c r="X5" s="123"/>
     </row>
     <row r="6" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="194">
+      <c r="B6" s="195">
         <v>5</v>
       </c>
-      <c r="C6" s="194"/>
-      <c r="D6" s="194"/>
-      <c r="E6" s="194"/>
-      <c r="F6" s="194"/>
+      <c r="C6" s="195"/>
+      <c r="D6" s="195"/>
+      <c r="E6" s="195"/>
+      <c r="F6" s="195"/>
       <c r="G6" s="123"/>
-      <c r="H6" s="194">
+      <c r="H6" s="195">
         <v>6</v>
       </c>
-      <c r="I6" s="194"/>
-      <c r="J6" s="194"/>
-      <c r="K6" s="194"/>
-      <c r="L6" s="194"/>
+      <c r="I6" s="195"/>
+      <c r="J6" s="195"/>
+      <c r="K6" s="195"/>
+      <c r="L6" s="195"/>
       <c r="M6" s="123"/>
-      <c r="N6" s="194">
+      <c r="N6" s="195">
         <v>7</v>
       </c>
-      <c r="O6" s="194"/>
-      <c r="P6" s="194"/>
-      <c r="Q6" s="194"/>
-      <c r="R6" s="194"/>
+      <c r="O6" s="195"/>
+      <c r="P6" s="195"/>
+      <c r="Q6" s="195"/>
+      <c r="R6" s="195"/>
       <c r="S6" s="123"/>
-      <c r="T6" s="194">
+      <c r="T6" s="195">
         <v>8</v>
       </c>
-      <c r="U6" s="194"/>
-      <c r="V6" s="194"/>
-      <c r="W6" s="194"/>
-      <c r="X6" s="194"/>
+      <c r="U6" s="195"/>
+      <c r="V6" s="195"/>
+      <c r="W6" s="195"/>
+      <c r="X6" s="195"/>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B7" s="105" t="s">
@@ -5780,37 +5793,37 @@
       <c r="X10" s="123"/>
     </row>
     <row r="11" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="194">
+      <c r="B11" s="195">
         <v>9</v>
       </c>
-      <c r="C11" s="194"/>
-      <c r="D11" s="194"/>
-      <c r="E11" s="194"/>
-      <c r="F11" s="194"/>
+      <c r="C11" s="195"/>
+      <c r="D11" s="195"/>
+      <c r="E11" s="195"/>
+      <c r="F11" s="195"/>
       <c r="G11" s="123"/>
-      <c r="H11" s="194">
+      <c r="H11" s="195">
         <v>10</v>
       </c>
-      <c r="I11" s="194"/>
-      <c r="J11" s="194"/>
-      <c r="K11" s="194"/>
-      <c r="L11" s="194"/>
+      <c r="I11" s="195"/>
+      <c r="J11" s="195"/>
+      <c r="K11" s="195"/>
+      <c r="L11" s="195"/>
       <c r="M11" s="123"/>
-      <c r="N11" s="194">
+      <c r="N11" s="195">
         <v>11</v>
       </c>
-      <c r="O11" s="194"/>
-      <c r="P11" s="194"/>
-      <c r="Q11" s="194"/>
-      <c r="R11" s="194"/>
+      <c r="O11" s="195"/>
+      <c r="P11" s="195"/>
+      <c r="Q11" s="195"/>
+      <c r="R11" s="195"/>
       <c r="S11" s="123"/>
-      <c r="T11" s="194">
+      <c r="T11" s="195">
         <v>12</v>
       </c>
-      <c r="U11" s="194"/>
-      <c r="V11" s="194"/>
-      <c r="W11" s="194"/>
-      <c r="X11" s="194"/>
+      <c r="U11" s="195"/>
+      <c r="V11" s="195"/>
+      <c r="W11" s="195"/>
+      <c r="X11" s="195"/>
     </row>
     <row r="12" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B12" s="105" t="s">
@@ -6033,37 +6046,37 @@
       <c r="X15" s="123"/>
     </row>
     <row r="16" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="194">
+      <c r="B16" s="195">
         <v>13</v>
       </c>
-      <c r="C16" s="194"/>
-      <c r="D16" s="194"/>
-      <c r="E16" s="194"/>
-      <c r="F16" s="194"/>
+      <c r="C16" s="195"/>
+      <c r="D16" s="195"/>
+      <c r="E16" s="195"/>
+      <c r="F16" s="195"/>
       <c r="G16" s="123"/>
-      <c r="H16" s="194">
+      <c r="H16" s="195">
         <v>14</v>
       </c>
-      <c r="I16" s="194"/>
-      <c r="J16" s="194"/>
-      <c r="K16" s="194"/>
-      <c r="L16" s="194"/>
+      <c r="I16" s="195"/>
+      <c r="J16" s="195"/>
+      <c r="K16" s="195"/>
+      <c r="L16" s="195"/>
       <c r="M16" s="123"/>
-      <c r="N16" s="194">
+      <c r="N16" s="195">
         <v>15</v>
       </c>
-      <c r="O16" s="194"/>
-      <c r="P16" s="194"/>
-      <c r="Q16" s="194"/>
-      <c r="R16" s="194"/>
+      <c r="O16" s="195"/>
+      <c r="P16" s="195"/>
+      <c r="Q16" s="195"/>
+      <c r="R16" s="195"/>
       <c r="S16" s="123"/>
-      <c r="T16" s="194">
+      <c r="T16" s="195">
         <v>16</v>
       </c>
-      <c r="U16" s="194"/>
-      <c r="V16" s="194"/>
-      <c r="W16" s="194"/>
-      <c r="X16" s="194"/>
+      <c r="U16" s="195"/>
+      <c r="V16" s="195"/>
+      <c r="W16" s="195"/>
+      <c r="X16" s="195"/>
     </row>
     <row r="17" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B17" s="105" t="s">
@@ -6261,34 +6274,34 @@
       </c>
     </row>
     <row r="21" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="193">
+      <c r="B21" s="194">
         <v>17</v>
       </c>
-      <c r="C21" s="193"/>
-      <c r="D21" s="193"/>
-      <c r="E21" s="193"/>
-      <c r="F21" s="193"/>
-      <c r="H21" s="193">
+      <c r="C21" s="194"/>
+      <c r="D21" s="194"/>
+      <c r="E21" s="194"/>
+      <c r="F21" s="194"/>
+      <c r="H21" s="194">
         <v>18</v>
       </c>
-      <c r="I21" s="193"/>
-      <c r="J21" s="193"/>
-      <c r="K21" s="193"/>
-      <c r="L21" s="193"/>
-      <c r="N21" s="193">
+      <c r="I21" s="194"/>
+      <c r="J21" s="194"/>
+      <c r="K21" s="194"/>
+      <c r="L21" s="194"/>
+      <c r="N21" s="194">
         <v>19</v>
       </c>
-      <c r="O21" s="193"/>
-      <c r="P21" s="193"/>
-      <c r="Q21" s="193"/>
-      <c r="R21" s="193"/>
-      <c r="T21" s="193">
+      <c r="O21" s="194"/>
+      <c r="P21" s="194"/>
+      <c r="Q21" s="194"/>
+      <c r="R21" s="194"/>
+      <c r="T21" s="194">
         <v>20</v>
       </c>
-      <c r="U21" s="193"/>
-      <c r="V21" s="193"/>
-      <c r="W21" s="193"/>
-      <c r="X21" s="193"/>
+      <c r="U21" s="194"/>
+      <c r="V21" s="194"/>
+      <c r="W21" s="194"/>
+      <c r="X21" s="194"/>
     </row>
     <row r="22" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B22" s="105" t="s">
@@ -6477,34 +6490,34 @@
       </c>
     </row>
     <row r="26" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="193">
-        <v>21</v>
-      </c>
-      <c r="C26" s="193"/>
-      <c r="D26" s="193"/>
-      <c r="E26" s="193"/>
-      <c r="F26" s="193"/>
-      <c r="H26" s="193">
+      <c r="B26" s="194">
+        <v>21</v>
+      </c>
+      <c r="C26" s="194"/>
+      <c r="D26" s="194"/>
+      <c r="E26" s="194"/>
+      <c r="F26" s="194"/>
+      <c r="H26" s="194">
         <v>22</v>
       </c>
-      <c r="I26" s="193"/>
-      <c r="J26" s="193"/>
-      <c r="K26" s="193"/>
-      <c r="L26" s="193"/>
-      <c r="N26" s="193">
+      <c r="I26" s="194"/>
+      <c r="J26" s="194"/>
+      <c r="K26" s="194"/>
+      <c r="L26" s="194"/>
+      <c r="N26" s="194">
         <v>23</v>
       </c>
-      <c r="O26" s="193"/>
-      <c r="P26" s="193"/>
-      <c r="Q26" s="193"/>
-      <c r="R26" s="193"/>
-      <c r="T26" s="193">
+      <c r="O26" s="194"/>
+      <c r="P26" s="194"/>
+      <c r="Q26" s="194"/>
+      <c r="R26" s="194"/>
+      <c r="T26" s="194">
         <v>24</v>
       </c>
-      <c r="U26" s="193"/>
-      <c r="V26" s="193"/>
-      <c r="W26" s="193"/>
-      <c r="X26" s="193"/>
+      <c r="U26" s="194"/>
+      <c r="V26" s="194"/>
+      <c r="W26" s="194"/>
+      <c r="X26" s="194"/>
     </row>
     <row r="27" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B27" s="105" t="s">
@@ -6693,13 +6706,13 @@
       </c>
     </row>
     <row r="31" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="193">
+      <c r="B31" s="194">
         <v>25</v>
       </c>
-      <c r="C31" s="193"/>
-      <c r="D31" s="193"/>
-      <c r="E31" s="193"/>
-      <c r="F31" s="193"/>
+      <c r="C31" s="194"/>
+      <c r="D31" s="194"/>
+      <c r="E31" s="194"/>
+      <c r="F31" s="194"/>
       <c r="H31" s="154"/>
       <c r="I31" s="154"/>
       <c r="J31" s="154"/>
@@ -6786,6 +6799,22 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="H1:L1"/>
+    <mergeCell ref="N1:R1"/>
+    <mergeCell ref="T1:X1"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="H6:L6"/>
+    <mergeCell ref="N6:R6"/>
+    <mergeCell ref="T6:X6"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="H11:L11"/>
+    <mergeCell ref="N11:R11"/>
+    <mergeCell ref="T11:X11"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="H16:L16"/>
+    <mergeCell ref="N16:R16"/>
+    <mergeCell ref="T16:X16"/>
     <mergeCell ref="B31:F31"/>
     <mergeCell ref="B21:F21"/>
     <mergeCell ref="H21:L21"/>
@@ -6795,22 +6824,6 @@
     <mergeCell ref="H26:L26"/>
     <mergeCell ref="N26:R26"/>
     <mergeCell ref="T26:X26"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="H11:L11"/>
-    <mergeCell ref="N11:R11"/>
-    <mergeCell ref="T11:X11"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="H16:L16"/>
-    <mergeCell ref="N16:R16"/>
-    <mergeCell ref="T16:X16"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="H1:L1"/>
-    <mergeCell ref="N1:R1"/>
-    <mergeCell ref="T1:X1"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="H6:L6"/>
-    <mergeCell ref="N6:R6"/>
-    <mergeCell ref="T6:X6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7450,33 +7463,33 @@
       <c r="S9" s="151">
         <v>0.01</v>
       </c>
-      <c r="T9" s="187" t="s">
+      <c r="T9" s="188" t="s">
         <v>75</v>
       </c>
-      <c r="U9" s="187"/>
-      <c r="V9" s="187"/>
-      <c r="W9" s="187"/>
-      <c r="X9" s="187"/>
-      <c r="Y9" s="187"/>
-      <c r="Z9" s="187"/>
-      <c r="AA9" s="187"/>
-      <c r="AB9" s="187"/>
-      <c r="AC9" s="187"/>
+      <c r="U9" s="188"/>
+      <c r="V9" s="188"/>
+      <c r="W9" s="188"/>
+      <c r="X9" s="188"/>
+      <c r="Y9" s="188"/>
+      <c r="Z9" s="188"/>
+      <c r="AA9" s="188"/>
+      <c r="AB9" s="188"/>
+      <c r="AC9" s="188"/>
       <c r="AE9" s="151">
         <v>0.01</v>
       </c>
-      <c r="AF9" s="187" t="s">
+      <c r="AF9" s="188" t="s">
         <v>76</v>
       </c>
-      <c r="AG9" s="187"/>
-      <c r="AH9" s="187"/>
-      <c r="AI9" s="187"/>
-      <c r="AJ9" s="187"/>
-      <c r="AK9" s="187"/>
-      <c r="AL9" s="187"/>
-      <c r="AM9" s="187"/>
-      <c r="AN9" s="187"/>
-      <c r="AO9" s="187"/>
+      <c r="AG9" s="188"/>
+      <c r="AH9" s="188"/>
+      <c r="AI9" s="188"/>
+      <c r="AJ9" s="188"/>
+      <c r="AK9" s="188"/>
+      <c r="AL9" s="188"/>
+      <c r="AM9" s="188"/>
+      <c r="AN9" s="188"/>
+      <c r="AO9" s="188"/>
     </row>
     <row r="10" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A10" s="101" t="s">
@@ -8766,44 +8779,44 @@
       <c r="G19" s="153">
         <v>0.03</v>
       </c>
-      <c r="H19" s="195"/>
-      <c r="I19" s="195"/>
-      <c r="J19" s="195"/>
-      <c r="K19" s="195"/>
-      <c r="L19" s="195"/>
-      <c r="M19" s="195"/>
-      <c r="N19" s="195"/>
-      <c r="O19" s="195"/>
-      <c r="P19" s="195"/>
-      <c r="Q19" s="195"/>
+      <c r="H19" s="197"/>
+      <c r="I19" s="197"/>
+      <c r="J19" s="197"/>
+      <c r="K19" s="197"/>
+      <c r="L19" s="197"/>
+      <c r="M19" s="197"/>
+      <c r="N19" s="197"/>
+      <c r="O19" s="197"/>
+      <c r="P19" s="197"/>
+      <c r="Q19" s="197"/>
       <c r="R19" s="152"/>
       <c r="S19" s="153">
         <v>0.03</v>
       </c>
-      <c r="T19" s="195"/>
-      <c r="U19" s="195"/>
-      <c r="V19" s="195"/>
-      <c r="W19" s="195"/>
-      <c r="X19" s="195"/>
-      <c r="Y19" s="195"/>
-      <c r="Z19" s="195"/>
-      <c r="AA19" s="195"/>
-      <c r="AB19" s="195"/>
-      <c r="AC19" s="195"/>
+      <c r="T19" s="197"/>
+      <c r="U19" s="197"/>
+      <c r="V19" s="197"/>
+      <c r="W19" s="197"/>
+      <c r="X19" s="197"/>
+      <c r="Y19" s="197"/>
+      <c r="Z19" s="197"/>
+      <c r="AA19" s="197"/>
+      <c r="AB19" s="197"/>
+      <c r="AC19" s="197"/>
       <c r="AD19" s="152"/>
       <c r="AE19" s="151">
         <v>0.03</v>
       </c>
-      <c r="AF19" s="195"/>
-      <c r="AG19" s="195"/>
-      <c r="AH19" s="195"/>
-      <c r="AI19" s="195"/>
-      <c r="AJ19" s="195"/>
-      <c r="AK19" s="195"/>
-      <c r="AL19" s="195"/>
-      <c r="AM19" s="195"/>
-      <c r="AN19" s="195"/>
-      <c r="AO19" s="195"/>
+      <c r="AF19" s="197"/>
+      <c r="AG19" s="197"/>
+      <c r="AH19" s="197"/>
+      <c r="AI19" s="197"/>
+      <c r="AJ19" s="197"/>
+      <c r="AK19" s="197"/>
+      <c r="AL19" s="197"/>
+      <c r="AM19" s="197"/>
+      <c r="AN19" s="197"/>
+      <c r="AO19" s="197"/>
     </row>
     <row r="20" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A20" s="97">
@@ -11258,44 +11271,44 @@
       <c r="G39" s="153">
         <v>0.1</v>
       </c>
-      <c r="H39" s="195"/>
-      <c r="I39" s="195"/>
-      <c r="J39" s="195"/>
-      <c r="K39" s="195"/>
-      <c r="L39" s="195"/>
-      <c r="M39" s="195"/>
-      <c r="N39" s="195"/>
-      <c r="O39" s="195"/>
-      <c r="P39" s="195"/>
-      <c r="Q39" s="195"/>
+      <c r="H39" s="197"/>
+      <c r="I39" s="197"/>
+      <c r="J39" s="197"/>
+      <c r="K39" s="197"/>
+      <c r="L39" s="197"/>
+      <c r="M39" s="197"/>
+      <c r="N39" s="197"/>
+      <c r="O39" s="197"/>
+      <c r="P39" s="197"/>
+      <c r="Q39" s="197"/>
       <c r="R39" s="152"/>
       <c r="S39" s="153">
         <v>0.1</v>
       </c>
-      <c r="T39" s="195"/>
-      <c r="U39" s="195"/>
-      <c r="V39" s="195"/>
-      <c r="W39" s="195"/>
-      <c r="X39" s="195"/>
-      <c r="Y39" s="195"/>
-      <c r="Z39" s="195"/>
-      <c r="AA39" s="195"/>
-      <c r="AB39" s="195"/>
-      <c r="AC39" s="195"/>
+      <c r="T39" s="197"/>
+      <c r="U39" s="197"/>
+      <c r="V39" s="197"/>
+      <c r="W39" s="197"/>
+      <c r="X39" s="197"/>
+      <c r="Y39" s="197"/>
+      <c r="Z39" s="197"/>
+      <c r="AA39" s="197"/>
+      <c r="AB39" s="197"/>
+      <c r="AC39" s="197"/>
       <c r="AD39" s="152"/>
       <c r="AE39" s="151">
         <v>0.1</v>
       </c>
-      <c r="AF39" s="195"/>
-      <c r="AG39" s="195"/>
-      <c r="AH39" s="195"/>
-      <c r="AI39" s="195"/>
-      <c r="AJ39" s="195"/>
-      <c r="AK39" s="195"/>
-      <c r="AL39" s="195"/>
-      <c r="AM39" s="195"/>
-      <c r="AN39" s="195"/>
-      <c r="AO39" s="195"/>
+      <c r="AF39" s="197"/>
+      <c r="AG39" s="197"/>
+      <c r="AH39" s="197"/>
+      <c r="AI39" s="197"/>
+      <c r="AJ39" s="197"/>
+      <c r="AK39" s="197"/>
+      <c r="AL39" s="197"/>
+      <c r="AM39" s="197"/>
+      <c r="AN39" s="197"/>
+      <c r="AO39" s="197"/>
     </row>
     <row r="40" spans="7:41" x14ac:dyDescent="0.25">
       <c r="G40" s="158">
@@ -13738,44 +13751,44 @@
       <c r="G59" s="153">
         <v>0.5</v>
       </c>
-      <c r="H59" s="195"/>
-      <c r="I59" s="195"/>
-      <c r="J59" s="195"/>
-      <c r="K59" s="195"/>
-      <c r="L59" s="195"/>
-      <c r="M59" s="195"/>
-      <c r="N59" s="195"/>
-      <c r="O59" s="195"/>
-      <c r="P59" s="195"/>
-      <c r="Q59" s="195"/>
+      <c r="H59" s="197"/>
+      <c r="I59" s="197"/>
+      <c r="J59" s="197"/>
+      <c r="K59" s="197"/>
+      <c r="L59" s="197"/>
+      <c r="M59" s="197"/>
+      <c r="N59" s="197"/>
+      <c r="O59" s="197"/>
+      <c r="P59" s="197"/>
+      <c r="Q59" s="197"/>
       <c r="R59" s="152"/>
       <c r="S59" s="153">
         <v>0.5</v>
       </c>
-      <c r="T59" s="195"/>
-      <c r="U59" s="195"/>
-      <c r="V59" s="195"/>
-      <c r="W59" s="195"/>
-      <c r="X59" s="195"/>
-      <c r="Y59" s="195"/>
-      <c r="Z59" s="195"/>
-      <c r="AA59" s="195"/>
-      <c r="AB59" s="195"/>
-      <c r="AC59" s="195"/>
+      <c r="T59" s="197"/>
+      <c r="U59" s="197"/>
+      <c r="V59" s="197"/>
+      <c r="W59" s="197"/>
+      <c r="X59" s="197"/>
+      <c r="Y59" s="197"/>
+      <c r="Z59" s="197"/>
+      <c r="AA59" s="197"/>
+      <c r="AB59" s="197"/>
+      <c r="AC59" s="197"/>
       <c r="AD59" s="152"/>
       <c r="AE59" s="151">
         <v>0.5</v>
       </c>
-      <c r="AF59" s="195"/>
-      <c r="AG59" s="195"/>
-      <c r="AH59" s="195"/>
-      <c r="AI59" s="195"/>
-      <c r="AJ59" s="195"/>
-      <c r="AK59" s="195"/>
-      <c r="AL59" s="195"/>
-      <c r="AM59" s="195"/>
-      <c r="AN59" s="195"/>
-      <c r="AO59" s="195"/>
+      <c r="AF59" s="197"/>
+      <c r="AG59" s="197"/>
+      <c r="AH59" s="197"/>
+      <c r="AI59" s="197"/>
+      <c r="AJ59" s="197"/>
+      <c r="AK59" s="197"/>
+      <c r="AL59" s="197"/>
+      <c r="AM59" s="197"/>
+      <c r="AN59" s="197"/>
+      <c r="AO59" s="197"/>
     </row>
     <row r="60" spans="7:41" x14ac:dyDescent="0.25">
       <c r="G60" s="158">
@@ -14976,11 +14989,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="H9:Q9"/>
-    <mergeCell ref="T9:AC9"/>
-    <mergeCell ref="AF9:AO9"/>
-    <mergeCell ref="AF19:AO19"/>
-    <mergeCell ref="AF39:AO39"/>
     <mergeCell ref="AF59:AO59"/>
     <mergeCell ref="T19:AC19"/>
     <mergeCell ref="T39:AC39"/>
@@ -14988,6 +14996,11 @@
     <mergeCell ref="H19:Q19"/>
     <mergeCell ref="H39:Q39"/>
     <mergeCell ref="H59:Q59"/>
+    <mergeCell ref="H9:Q9"/>
+    <mergeCell ref="T9:AC9"/>
+    <mergeCell ref="AF9:AO9"/>
+    <mergeCell ref="AF19:AO19"/>
+    <mergeCell ref="AF39:AO39"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="AF20:AO28 AF60:AO68 AF40:AO48">
@@ -18202,34 +18215,34 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="193">
-        <v>1</v>
-      </c>
-      <c r="C1" s="193"/>
-      <c r="D1" s="193"/>
-      <c r="E1" s="193"/>
-      <c r="F1" s="193"/>
-      <c r="H1" s="193">
-        <v>2</v>
-      </c>
-      <c r="I1" s="193"/>
-      <c r="J1" s="193"/>
-      <c r="K1" s="193"/>
-      <c r="L1" s="193"/>
-      <c r="N1" s="193">
+      <c r="B1" s="194">
+        <v>1</v>
+      </c>
+      <c r="C1" s="194"/>
+      <c r="D1" s="194"/>
+      <c r="E1" s="194"/>
+      <c r="F1" s="194"/>
+      <c r="H1" s="194">
+        <v>2</v>
+      </c>
+      <c r="I1" s="194"/>
+      <c r="J1" s="194"/>
+      <c r="K1" s="194"/>
+      <c r="L1" s="194"/>
+      <c r="N1" s="194">
         <v>3</v>
       </c>
-      <c r="O1" s="193"/>
-      <c r="P1" s="193"/>
-      <c r="Q1" s="193"/>
-      <c r="R1" s="193"/>
-      <c r="T1" s="193">
+      <c r="O1" s="194"/>
+      <c r="P1" s="194"/>
+      <c r="Q1" s="194"/>
+      <c r="R1" s="194"/>
+      <c r="T1" s="194">
         <v>4</v>
       </c>
-      <c r="U1" s="193"/>
-      <c r="V1" s="193"/>
-      <c r="W1" s="193"/>
-      <c r="X1" s="193"/>
+      <c r="U1" s="194"/>
+      <c r="V1" s="194"/>
+      <c r="W1" s="194"/>
+      <c r="X1" s="194"/>
     </row>
     <row r="2" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B2" s="39"/>
@@ -18298,34 +18311,34 @@
       <c r="X4" s="46"/>
     </row>
     <row r="6" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="193">
+      <c r="B6" s="194">
         <v>5</v>
       </c>
-      <c r="C6" s="193"/>
-      <c r="D6" s="193"/>
-      <c r="E6" s="193"/>
-      <c r="F6" s="193"/>
-      <c r="H6" s="193">
+      <c r="C6" s="194"/>
+      <c r="D6" s="194"/>
+      <c r="E6" s="194"/>
+      <c r="F6" s="194"/>
+      <c r="H6" s="194">
         <v>6</v>
       </c>
-      <c r="I6" s="193"/>
-      <c r="J6" s="193"/>
-      <c r="K6" s="193"/>
-      <c r="L6" s="193"/>
-      <c r="N6" s="193">
+      <c r="I6" s="194"/>
+      <c r="J6" s="194"/>
+      <c r="K6" s="194"/>
+      <c r="L6" s="194"/>
+      <c r="N6" s="194">
         <v>7</v>
       </c>
-      <c r="O6" s="193"/>
-      <c r="P6" s="193"/>
-      <c r="Q6" s="193"/>
-      <c r="R6" s="193"/>
-      <c r="T6" s="193">
+      <c r="O6" s="194"/>
+      <c r="P6" s="194"/>
+      <c r="Q6" s="194"/>
+      <c r="R6" s="194"/>
+      <c r="T6" s="194">
         <v>8</v>
       </c>
-      <c r="U6" s="193"/>
-      <c r="V6" s="193"/>
-      <c r="W6" s="193"/>
-      <c r="X6" s="193"/>
+      <c r="U6" s="194"/>
+      <c r="V6" s="194"/>
+      <c r="W6" s="194"/>
+      <c r="X6" s="194"/>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B7" s="39"/>
@@ -18394,34 +18407,34 @@
       <c r="X9" s="59"/>
     </row>
     <row r="11" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="193">
+      <c r="B11" s="194">
         <v>9</v>
       </c>
-      <c r="C11" s="193"/>
-      <c r="D11" s="193"/>
-      <c r="E11" s="193"/>
-      <c r="F11" s="193"/>
-      <c r="H11" s="193">
+      <c r="C11" s="194"/>
+      <c r="D11" s="194"/>
+      <c r="E11" s="194"/>
+      <c r="F11" s="194"/>
+      <c r="H11" s="194">
         <v>10</v>
       </c>
-      <c r="I11" s="193"/>
-      <c r="J11" s="193"/>
-      <c r="K11" s="193"/>
-      <c r="L11" s="193"/>
-      <c r="N11" s="193">
+      <c r="I11" s="194"/>
+      <c r="J11" s="194"/>
+      <c r="K11" s="194"/>
+      <c r="L11" s="194"/>
+      <c r="N11" s="194">
         <v>11</v>
       </c>
-      <c r="O11" s="193"/>
-      <c r="P11" s="193"/>
-      <c r="Q11" s="193"/>
-      <c r="R11" s="193"/>
-      <c r="T11" s="193">
+      <c r="O11" s="194"/>
+      <c r="P11" s="194"/>
+      <c r="Q11" s="194"/>
+      <c r="R11" s="194"/>
+      <c r="T11" s="194">
         <v>12</v>
       </c>
-      <c r="U11" s="193"/>
-      <c r="V11" s="193"/>
-      <c r="W11" s="193"/>
-      <c r="X11" s="193"/>
+      <c r="U11" s="194"/>
+      <c r="V11" s="194"/>
+      <c r="W11" s="194"/>
+      <c r="X11" s="194"/>
     </row>
     <row r="12" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B12" s="39"/>
@@ -18490,34 +18503,34 @@
       <c r="X14" s="46"/>
     </row>
     <row r="16" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="193">
+      <c r="B16" s="194">
         <v>13</v>
       </c>
-      <c r="C16" s="193"/>
-      <c r="D16" s="193"/>
-      <c r="E16" s="193"/>
-      <c r="F16" s="193"/>
-      <c r="H16" s="193">
+      <c r="C16" s="194"/>
+      <c r="D16" s="194"/>
+      <c r="E16" s="194"/>
+      <c r="F16" s="194"/>
+      <c r="H16" s="194">
         <v>14</v>
       </c>
-      <c r="I16" s="193"/>
-      <c r="J16" s="193"/>
-      <c r="K16" s="193"/>
-      <c r="L16" s="193"/>
-      <c r="N16" s="193">
+      <c r="I16" s="194"/>
+      <c r="J16" s="194"/>
+      <c r="K16" s="194"/>
+      <c r="L16" s="194"/>
+      <c r="N16" s="194">
         <v>15</v>
       </c>
-      <c r="O16" s="193"/>
-      <c r="P16" s="193"/>
-      <c r="Q16" s="193"/>
-      <c r="R16" s="193"/>
-      <c r="T16" s="193">
+      <c r="O16" s="194"/>
+      <c r="P16" s="194"/>
+      <c r="Q16" s="194"/>
+      <c r="R16" s="194"/>
+      <c r="T16" s="194">
         <v>16</v>
       </c>
-      <c r="U16" s="193"/>
-      <c r="V16" s="193"/>
-      <c r="W16" s="193"/>
-      <c r="X16" s="193"/>
+      <c r="U16" s="194"/>
+      <c r="V16" s="194"/>
+      <c r="W16" s="194"/>
+      <c r="X16" s="194"/>
     </row>
     <row r="17" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B17" s="39"/>
@@ -18586,34 +18599,34 @@
       <c r="X19" s="46"/>
     </row>
     <row r="21" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="193">
+      <c r="B21" s="194">
         <v>17</v>
       </c>
-      <c r="C21" s="193"/>
-      <c r="D21" s="193"/>
-      <c r="E21" s="193"/>
-      <c r="F21" s="193"/>
-      <c r="H21" s="193">
+      <c r="C21" s="194"/>
+      <c r="D21" s="194"/>
+      <c r="E21" s="194"/>
+      <c r="F21" s="194"/>
+      <c r="H21" s="194">
         <v>18</v>
       </c>
-      <c r="I21" s="193"/>
-      <c r="J21" s="193"/>
-      <c r="K21" s="193"/>
-      <c r="L21" s="193"/>
-      <c r="N21" s="193">
+      <c r="I21" s="194"/>
+      <c r="J21" s="194"/>
+      <c r="K21" s="194"/>
+      <c r="L21" s="194"/>
+      <c r="N21" s="194">
         <v>19</v>
       </c>
-      <c r="O21" s="193"/>
-      <c r="P21" s="193"/>
-      <c r="Q21" s="193"/>
-      <c r="R21" s="193"/>
-      <c r="T21" s="193">
+      <c r="O21" s="194"/>
+      <c r="P21" s="194"/>
+      <c r="Q21" s="194"/>
+      <c r="R21" s="194"/>
+      <c r="T21" s="194">
         <v>20</v>
       </c>
-      <c r="U21" s="193"/>
-      <c r="V21" s="193"/>
-      <c r="W21" s="193"/>
-      <c r="X21" s="193"/>
+      <c r="U21" s="194"/>
+      <c r="V21" s="194"/>
+      <c r="W21" s="194"/>
+      <c r="X21" s="194"/>
     </row>
     <row r="22" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B22" s="39"/>
@@ -18682,34 +18695,34 @@
       <c r="X24" s="46"/>
     </row>
     <row r="26" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="193">
-        <v>21</v>
-      </c>
-      <c r="C26" s="193"/>
-      <c r="D26" s="193"/>
-      <c r="E26" s="193"/>
-      <c r="F26" s="193"/>
-      <c r="H26" s="193">
+      <c r="B26" s="194">
+        <v>21</v>
+      </c>
+      <c r="C26" s="194"/>
+      <c r="D26" s="194"/>
+      <c r="E26" s="194"/>
+      <c r="F26" s="194"/>
+      <c r="H26" s="194">
         <v>22</v>
       </c>
-      <c r="I26" s="193"/>
-      <c r="J26" s="193"/>
-      <c r="K26" s="193"/>
-      <c r="L26" s="193"/>
-      <c r="N26" s="193">
+      <c r="I26" s="194"/>
+      <c r="J26" s="194"/>
+      <c r="K26" s="194"/>
+      <c r="L26" s="194"/>
+      <c r="N26" s="194">
         <v>23</v>
       </c>
-      <c r="O26" s="193"/>
-      <c r="P26" s="193"/>
-      <c r="Q26" s="193"/>
-      <c r="R26" s="193"/>
-      <c r="T26" s="193">
+      <c r="O26" s="194"/>
+      <c r="P26" s="194"/>
+      <c r="Q26" s="194"/>
+      <c r="R26" s="194"/>
+      <c r="T26" s="194">
         <v>24</v>
       </c>
-      <c r="U26" s="193"/>
-      <c r="V26" s="193"/>
-      <c r="W26" s="193"/>
-      <c r="X26" s="193"/>
+      <c r="U26" s="194"/>
+      <c r="V26" s="194"/>
+      <c r="W26" s="194"/>
+      <c r="X26" s="194"/>
     </row>
     <row r="27" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B27" s="39"/>
@@ -18778,13 +18791,13 @@
       <c r="X29" s="46"/>
     </row>
     <row r="31" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="193">
+      <c r="B31" s="194">
         <v>25</v>
       </c>
-      <c r="C31" s="193"/>
-      <c r="D31" s="193"/>
-      <c r="E31" s="193"/>
-      <c r="F31" s="193"/>
+      <c r="C31" s="194"/>
+      <c r="D31" s="194"/>
+      <c r="E31" s="194"/>
+      <c r="F31" s="194"/>
     </row>
     <row r="32" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B32" s="39"/>
@@ -18809,6 +18822,22 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="H1:L1"/>
+    <mergeCell ref="N1:R1"/>
+    <mergeCell ref="T1:X1"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="H6:L6"/>
+    <mergeCell ref="N6:R6"/>
+    <mergeCell ref="T6:X6"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="H11:L11"/>
+    <mergeCell ref="N11:R11"/>
+    <mergeCell ref="T11:X11"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="H26:L26"/>
+    <mergeCell ref="N26:R26"/>
+    <mergeCell ref="T26:X26"/>
     <mergeCell ref="B31:F31"/>
     <mergeCell ref="T16:X16"/>
     <mergeCell ref="B21:F21"/>
@@ -18818,22 +18847,6 @@
     <mergeCell ref="B16:F16"/>
     <mergeCell ref="H16:L16"/>
     <mergeCell ref="N16:R16"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="H11:L11"/>
-    <mergeCell ref="N11:R11"/>
-    <mergeCell ref="T11:X11"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="H26:L26"/>
-    <mergeCell ref="N26:R26"/>
-    <mergeCell ref="T26:X26"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="H1:L1"/>
-    <mergeCell ref="N1:R1"/>
-    <mergeCell ref="T1:X1"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="H6:L6"/>
-    <mergeCell ref="N6:R6"/>
-    <mergeCell ref="T6:X6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -18857,40 +18870,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="197" t="s">
+      <c r="A1" s="198" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="198"/>
-      <c r="C1" s="198"/>
-      <c r="D1" s="199"/>
-      <c r="F1" s="197" t="s">
+      <c r="B1" s="199"/>
+      <c r="C1" s="199"/>
+      <c r="D1" s="200"/>
+      <c r="F1" s="198" t="s">
         <v>58</v>
       </c>
-      <c r="G1" s="198"/>
-      <c r="H1" s="199"/>
+      <c r="G1" s="199"/>
+      <c r="H1" s="200"/>
       <c r="I1" s="47"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="176" t="s">
+      <c r="A2" s="177" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="177"/>
-      <c r="C2" s="177"/>
-      <c r="D2" s="178"/>
-      <c r="F2" s="176" t="s">
+      <c r="B2" s="178"/>
+      <c r="C2" s="178"/>
+      <c r="D2" s="179"/>
+      <c r="F2" s="177" t="s">
         <v>59</v>
       </c>
-      <c r="G2" s="177"/>
-      <c r="H2" s="178"/>
+      <c r="G2" s="178"/>
+      <c r="H2" s="179"/>
       <c r="I2" s="47"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="176" t="s">
+      <c r="A3" s="177" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="177"/>
-      <c r="C3" s="177"/>
-      <c r="D3" s="178"/>
+      <c r="B3" s="178"/>
+      <c r="C3" s="178"/>
+      <c r="D3" s="179"/>
       <c r="F3" s="13" t="s">
         <v>60</v>
       </c>
@@ -19042,10 +19055,10 @@
       <c r="B12" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="179" t="s">
+      <c r="C12" s="180" t="s">
         <v>56</v>
       </c>
-      <c r="D12" s="180"/>
+      <c r="D12" s="181"/>
       <c r="F12" s="13" t="s">
         <v>67</v>
       </c>
@@ -19064,11 +19077,11 @@
       <c r="H13" s="66"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="176" t="s">
+      <c r="A14" s="177" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="177"/>
-      <c r="C14" s="177"/>
+      <c r="B14" s="178"/>
+      <c r="C14" s="178"/>
       <c r="D14" s="66"/>
       <c r="F14" s="13" t="s">
         <v>68</v>
@@ -19077,11 +19090,11 @@
       <c r="H14" s="66"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="176" t="s">
+      <c r="A15" s="177" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="177"/>
-      <c r="C15" s="177"/>
+      <c r="B15" s="178"/>
+      <c r="C15" s="178"/>
       <c r="D15" s="66"/>
       <c r="F15" s="13" t="s">
         <v>69</v>
@@ -19143,8 +19156,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DF38956-FDBF-4967-97AF-72744B5458AB}">
   <dimension ref="A1:AC174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H191" sqref="H191"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19276,11 +19289,11 @@
       <c r="P4" s="123" t="s">
         <v>21</v>
       </c>
-      <c r="Q4" s="200" t="s">
+      <c r="Q4" s="201" t="s">
         <v>185</v>
       </c>
-      <c r="R4" s="200"/>
-      <c r="S4" s="200"/>
+      <c r="R4" s="201"/>
+      <c r="S4" s="201"/>
     </row>
     <row r="5" spans="5:29" x14ac:dyDescent="0.25">
       <c r="E5" s="5"/>
@@ -19541,13 +19554,13 @@
       <c r="Q19" s="123"/>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A20" s="201" t="s">
+      <c r="A20" s="202" t="s">
         <v>200</v>
       </c>
-      <c r="B20" s="201"/>
-      <c r="C20" s="201"/>
-      <c r="D20" s="201"/>
-      <c r="E20" s="201"/>
+      <c r="B20" s="202"/>
+      <c r="C20" s="202"/>
+      <c r="D20" s="202"/>
+      <c r="E20" s="202"/>
       <c r="G20" s="1"/>
       <c r="M20" s="123"/>
       <c r="N20" s="123"/>

</xml_diff>